<commit_message>
Cambios visuales y graficos
</commit_message>
<xml_diff>
--- a/CMPC_Manufacturing/OutputCMPC.xlsx
+++ b/CMPC_Manufacturing/OutputCMPC.xlsx
@@ -693,13 +693,13 @@
         <v>9406.0</v>
       </c>
       <c r="L13" t="n">
-        <v>5346000.0</v>
+        <v>0.0</v>
       </c>
       <c r="M13" t="n">
         <v>43301.07631999999</v>
       </c>
       <c r="N13" t="n">
-        <v>0.008099714986906096</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
@@ -1245,13 +1245,13 @@
         <v>8704.0</v>
       </c>
       <c r="L25" t="n">
-        <v>5238000.0</v>
+        <v>0.0</v>
       </c>
       <c r="M25" t="n">
         <v>59546.61447999999</v>
       </c>
       <c r="N25" t="n">
-        <v>0.011368196731576935</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26">
@@ -14471,97 +14471,97 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>091-CH-TA-5·PRE-5·XX-96</t>
+          <t>552-UY-TA-5·PRE-5·XX-96</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c r="C24" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>AR-1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F24" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="G24" t="n">
-        <v>5346000.0</v>
+        <v>0.0</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0</v>
+        <v>7074000.0</v>
       </c>
       <c r="I24" t="n">
-        <v>418.3098591549278</v>
+        <v>0.0</v>
       </c>
       <c r="J24" t="n">
-        <v>418.3098591549278</v>
+        <v>0.0</v>
       </c>
       <c r="K24" t="n">
-        <v>0.10227442708333333</v>
+        <v>0.0</v>
       </c>
       <c r="L24" t="n">
-        <v>0.008099714986906096</v>
+        <v>0.0</v>
       </c>
       <c r="M24" t="n">
-        <v>0.11037414207023942</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>091-CH-TA-5·PRE-5·XX-96</t>
+          <t>566-UY-TA-3·ULT-5·XX-96</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c r="C25" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>AR-2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="F25" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="G25" t="n">
-        <v>5238000.0</v>
+        <v>0.0</v>
       </c>
       <c r="H25" t="n">
-        <v>0.0</v>
+        <v>7074000.0</v>
       </c>
       <c r="I25" t="n">
-        <v>351.30784708249234</v>
+        <v>0.0</v>
       </c>
       <c r="J25" t="n">
-        <v>351.30784708249234</v>
+        <v>0.0</v>
       </c>
       <c r="K25" t="n">
-        <v>0.103351</v>
+        <v>0.0</v>
       </c>
       <c r="L25" t="n">
-        <v>0.011368196731576935</v>
+        <v>0.0</v>
       </c>
       <c r="M25" t="n">
-        <v>0.11471919673157693</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>552-UY-TA-5·PRE-5·XX-96</t>
+          <t>123-CO-ST-4·ULP-4·XG-100</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -14606,7 +14606,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>566-UY-TA-3·ULT-5·XX-96</t>
+          <t>137-CO-ST-9·PVL-4·XG-100</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -14651,7 +14651,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>123-CO-ST-4·ULP-4·XG-100</t>
+          <t>152-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -14696,7 +14696,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>137-CO-ST-9·PVL-4·XG-100</t>
+          <t>153-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -14741,7 +14741,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>152-EC-TA-5·PRE-4·XG-100</t>
+          <t>166-EC-TA-3·ULT-4·XG-100</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -14786,7 +14786,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>153-EC-TA-5·PRE-4·XG-100</t>
+          <t>096-CH-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -14831,7 +14831,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>166-EC-TA-3·ULT-4·XG-100</t>
+          <t>555-UY-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -14876,7 +14876,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>096-CH-TA-5·PRE-4·XG-96</t>
+          <t>569-UY-TA-3·ULT-4·XG-96</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -14921,7 +14921,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>555-UY-TA-5·PRE-4·XG-96</t>
+          <t>122-CO-ST-4·ULP-3·GR-100</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -14966,7 +14966,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>569-UY-TA-3·ULT-4·XG-96</t>
+          <t>136-CO-ST-9·PVL-3·GR-100</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -15011,7 +15011,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>122-CO-ST-4·ULP-3·GR-100</t>
+          <t>148-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -15056,7 +15056,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>136-CO-ST-9·PVL-3·GR-100</t>
+          <t>149-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -15101,7 +15101,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>148-EC-TA-5·PRE-3·GR-100</t>
+          <t>163-EC-TA-3·ULT-3·GR-100</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -15146,7 +15146,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>149-EC-TA-5·PRE-3·GR-100</t>
+          <t>104-CH-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -15191,7 +15191,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>163-EC-TA-3·ULT-3·GR-100</t>
+          <t>121-CO-ST-4·ULP-2·MD-100</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -15236,7 +15236,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>104-CH-TA-5·PRE-2·MD-100</t>
+          <t>135-CO-ST-9·PVL-2·MD-100</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -15281,7 +15281,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>121-CO-ST-4·ULP-2·MD-100</t>
+          <t>144-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -15326,7 +15326,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>135-CO-ST-9·PVL-2·MD-100</t>
+          <t>145-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -15371,7 +15371,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>144-EC-TA-5·PRE-2·MD-100</t>
+          <t>160-EC-TA-3·ULT-2·MD-100</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -15416,7 +15416,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>145-EC-TA-5·PRE-2·MD-100</t>
+          <t>134-CO-TA-9·PVL-1·PQ-100</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -15461,11 +15461,11 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>160-EC-TA-3·ULT-2·MD-100</t>
+          <t>552-UY-TA-5·PRE-5·XX-96</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C46" t="n">
         <v>8.0</v>
@@ -15485,7 +15485,7 @@
         <v>0.0</v>
       </c>
       <c r="H46" t="n">
-        <v>7074000.0</v>
+        <v>1.2384E7</v>
       </c>
       <c r="I46" t="n">
         <v>0.0</v>
@@ -15506,11 +15506,11 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>134-CO-TA-9·PVL-1·PQ-100</t>
+          <t>566-UY-TA-3·ULT-5·XX-96</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C47" t="n">
         <v>8.0</v>
@@ -15530,7 +15530,7 @@
         <v>0.0</v>
       </c>
       <c r="H47" t="n">
-        <v>7074000.0</v>
+        <v>1.2384E7</v>
       </c>
       <c r="I47" t="n">
         <v>0.0</v>
@@ -15551,7 +15551,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>552-UY-TA-5·PRE-5·XX-96</t>
+          <t>123-CO-ST-4·ULP-4·XG-100</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -15596,7 +15596,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>566-UY-TA-3·ULT-5·XX-96</t>
+          <t>137-CO-ST-9·PVL-4·XG-100</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -15641,7 +15641,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>123-CO-ST-4·ULP-4·XG-100</t>
+          <t>152-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -15686,7 +15686,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>137-CO-ST-9·PVL-4·XG-100</t>
+          <t>153-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -15731,7 +15731,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>152-EC-TA-5·PRE-4·XG-100</t>
+          <t>166-EC-TA-3·ULT-4·XG-100</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -15776,7 +15776,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>153-EC-TA-5·PRE-4·XG-100</t>
+          <t>096-CH-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -15821,7 +15821,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>166-EC-TA-3·ULT-4·XG-100</t>
+          <t>555-UY-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -15866,7 +15866,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>096-CH-TA-5·PRE-4·XG-96</t>
+          <t>569-UY-TA-3·ULT-4·XG-96</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -15911,7 +15911,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>555-UY-TA-5·PRE-4·XG-96</t>
+          <t>122-CO-ST-4·ULP-3·GR-100</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -15956,7 +15956,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>569-UY-TA-3·ULT-4·XG-96</t>
+          <t>136-CO-ST-9·PVL-3·GR-100</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -16001,7 +16001,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>122-CO-ST-4·ULP-3·GR-100</t>
+          <t>148-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -16046,7 +16046,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>136-CO-ST-9·PVL-3·GR-100</t>
+          <t>149-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -16091,7 +16091,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>148-EC-TA-5·PRE-3·GR-100</t>
+          <t>163-EC-TA-3·ULT-3·GR-100</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -16136,7 +16136,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>149-EC-TA-5·PRE-3·GR-100</t>
+          <t>104-CH-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -16181,7 +16181,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>163-EC-TA-3·ULT-3·GR-100</t>
+          <t>121-CO-ST-4·ULP-2·MD-100</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -16226,7 +16226,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>104-CH-TA-5·PRE-2·MD-100</t>
+          <t>135-CO-ST-9·PVL-2·MD-100</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -16271,7 +16271,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>121-CO-ST-4·ULP-2·MD-100</t>
+          <t>144-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -16316,7 +16316,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>135-CO-ST-9·PVL-2·MD-100</t>
+          <t>145-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -16361,7 +16361,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>144-EC-TA-5·PRE-2·MD-100</t>
+          <t>160-EC-TA-3·ULT-2·MD-100</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -16406,7 +16406,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>145-EC-TA-5·PRE-2·MD-100</t>
+          <t>134-CO-TA-9·PVL-1·PQ-100</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -16451,11 +16451,11 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>160-EC-TA-3·ULT-2·MD-100</t>
+          <t>552-UY-TA-5·PRE-5·XX-96</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C68" t="n">
         <v>8.0</v>
@@ -16475,7 +16475,7 @@
         <v>0.0</v>
       </c>
       <c r="H68" t="n">
-        <v>1.2384E7</v>
+        <v>1.7676E7</v>
       </c>
       <c r="I68" t="n">
         <v>0.0</v>
@@ -16496,11 +16496,11 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>134-CO-TA-9·PVL-1·PQ-100</t>
+          <t>566-UY-TA-3·ULT-5·XX-96</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C69" t="n">
         <v>8.0</v>
@@ -16520,7 +16520,7 @@
         <v>0.0</v>
       </c>
       <c r="H69" t="n">
-        <v>1.2384E7</v>
+        <v>1.7676E7</v>
       </c>
       <c r="I69" t="n">
         <v>0.0</v>
@@ -16541,7 +16541,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>552-UY-TA-5·PRE-5·XX-96</t>
+          <t>123-CO-ST-4·ULP-4·XG-100</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -16586,7 +16586,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>566-UY-TA-3·ULT-5·XX-96</t>
+          <t>137-CO-ST-9·PVL-4·XG-100</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -16631,7 +16631,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>123-CO-ST-4·ULP-4·XG-100</t>
+          <t>152-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -16676,7 +16676,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>137-CO-ST-9·PVL-4·XG-100</t>
+          <t>153-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -16721,7 +16721,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>152-EC-TA-5·PRE-4·XG-100</t>
+          <t>166-EC-TA-3·ULT-4·XG-100</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -16766,7 +16766,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>153-EC-TA-5·PRE-4·XG-100</t>
+          <t>096-CH-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -16811,7 +16811,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>166-EC-TA-3·ULT-4·XG-100</t>
+          <t>555-UY-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -16856,7 +16856,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>096-CH-TA-5·PRE-4·XG-96</t>
+          <t>569-UY-TA-3·ULT-4·XG-96</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -16901,7 +16901,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>555-UY-TA-5·PRE-4·XG-96</t>
+          <t>122-CO-ST-4·ULP-3·GR-100</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -16946,7 +16946,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>569-UY-TA-3·ULT-4·XG-96</t>
+          <t>136-CO-ST-9·PVL-3·GR-100</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -16991,7 +16991,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>122-CO-ST-4·ULP-3·GR-100</t>
+          <t>148-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -17036,7 +17036,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>136-CO-ST-9·PVL-3·GR-100</t>
+          <t>149-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -17081,7 +17081,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>148-EC-TA-5·PRE-3·GR-100</t>
+          <t>163-EC-TA-3·ULT-3·GR-100</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -17126,7 +17126,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>149-EC-TA-5·PRE-3·GR-100</t>
+          <t>104-CH-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -17171,7 +17171,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>163-EC-TA-3·ULT-3·GR-100</t>
+          <t>121-CO-ST-4·ULP-2·MD-100</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -17216,7 +17216,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>104-CH-TA-5·PRE-2·MD-100</t>
+          <t>135-CO-ST-9·PVL-2·MD-100</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -17261,7 +17261,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>121-CO-ST-4·ULP-2·MD-100</t>
+          <t>144-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -17306,7 +17306,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>135-CO-ST-9·PVL-2·MD-100</t>
+          <t>145-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -17351,7 +17351,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>144-EC-TA-5·PRE-2·MD-100</t>
+          <t>160-EC-TA-3·ULT-2·MD-100</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -17396,7 +17396,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>145-EC-TA-5·PRE-2·MD-100</t>
+          <t>134-CO-TA-9·PVL-1·PQ-100</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -17441,11 +17441,11 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>160-EC-TA-3·ULT-2·MD-100</t>
+          <t>552-UY-TA-5·PRE-5·XX-96</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C90" t="n">
         <v>8.0</v>
@@ -17465,7 +17465,7 @@
         <v>0.0</v>
       </c>
       <c r="H90" t="n">
-        <v>1.7676E7</v>
+        <v>2.2968E7</v>
       </c>
       <c r="I90" t="n">
         <v>0.0</v>
@@ -17486,11 +17486,11 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>134-CO-TA-9·PVL-1·PQ-100</t>
+          <t>566-UY-TA-3·ULT-5·XX-96</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C91" t="n">
         <v>8.0</v>
@@ -17510,7 +17510,7 @@
         <v>0.0</v>
       </c>
       <c r="H91" t="n">
-        <v>1.7676E7</v>
+        <v>2.2968E7</v>
       </c>
       <c r="I91" t="n">
         <v>0.0</v>
@@ -17531,7 +17531,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>552-UY-TA-5·PRE-5·XX-96</t>
+          <t>123-CO-ST-4·ULP-4·XG-100</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -17576,7 +17576,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>566-UY-TA-3·ULT-5·XX-96</t>
+          <t>137-CO-ST-9·PVL-4·XG-100</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -17621,7 +17621,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>123-CO-ST-4·ULP-4·XG-100</t>
+          <t>152-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -17666,7 +17666,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>137-CO-ST-9·PVL-4·XG-100</t>
+          <t>153-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -17711,7 +17711,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>152-EC-TA-5·PRE-4·XG-100</t>
+          <t>166-EC-TA-3·ULT-4·XG-100</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -17756,7 +17756,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>153-EC-TA-5·PRE-4·XG-100</t>
+          <t>096-CH-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -17801,7 +17801,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>166-EC-TA-3·ULT-4·XG-100</t>
+          <t>555-UY-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -17846,7 +17846,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>096-CH-TA-5·PRE-4·XG-96</t>
+          <t>569-UY-TA-3·ULT-4·XG-96</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -17891,7 +17891,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>555-UY-TA-5·PRE-4·XG-96</t>
+          <t>122-CO-ST-4·ULP-3·GR-100</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -17936,7 +17936,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>569-UY-TA-3·ULT-4·XG-96</t>
+          <t>136-CO-ST-9·PVL-3·GR-100</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -17981,7 +17981,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>122-CO-ST-4·ULP-3·GR-100</t>
+          <t>148-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -18026,7 +18026,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>136-CO-ST-9·PVL-3·GR-100</t>
+          <t>149-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -18071,7 +18071,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>148-EC-TA-5·PRE-3·GR-100</t>
+          <t>163-EC-TA-3·ULT-3·GR-100</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -18116,7 +18116,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>149-EC-TA-5·PRE-3·GR-100</t>
+          <t>104-CH-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -18161,7 +18161,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>163-EC-TA-3·ULT-3·GR-100</t>
+          <t>121-CO-ST-4·ULP-2·MD-100</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -18206,7 +18206,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>104-CH-TA-5·PRE-2·MD-100</t>
+          <t>135-CO-ST-9·PVL-2·MD-100</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -18251,7 +18251,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>121-CO-ST-4·ULP-2·MD-100</t>
+          <t>144-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -18296,7 +18296,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>135-CO-ST-9·PVL-2·MD-100</t>
+          <t>145-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -18341,7 +18341,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>144-EC-TA-5·PRE-2·MD-100</t>
+          <t>160-EC-TA-3·ULT-2·MD-100</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -18386,7 +18386,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>145-EC-TA-5·PRE-2·MD-100</t>
+          <t>134-CO-TA-9·PVL-1·PQ-100</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -18431,11 +18431,11 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>160-EC-TA-3·ULT-2·MD-100</t>
+          <t>552-UY-TA-5·PRE-5·XX-96</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C112" t="n">
         <v>8.0</v>
@@ -18455,7 +18455,7 @@
         <v>0.0</v>
       </c>
       <c r="H112" t="n">
-        <v>2.2968E7</v>
+        <v>2.8278E7</v>
       </c>
       <c r="I112" t="n">
         <v>0.0</v>
@@ -18476,11 +18476,11 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>134-CO-TA-9·PVL-1·PQ-100</t>
+          <t>566-UY-TA-3·ULT-5·XX-96</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C113" t="n">
         <v>8.0</v>
@@ -18500,7 +18500,7 @@
         <v>0.0</v>
       </c>
       <c r="H113" t="n">
-        <v>2.2968E7</v>
+        <v>2.8278E7</v>
       </c>
       <c r="I113" t="n">
         <v>0.0</v>
@@ -18521,7 +18521,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>552-UY-TA-5·PRE-5·XX-96</t>
+          <t>123-CO-ST-4·ULP-4·XG-100</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -18566,7 +18566,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>566-UY-TA-3·ULT-5·XX-96</t>
+          <t>137-CO-ST-9·PVL-4·XG-100</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -18611,7 +18611,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>123-CO-ST-4·ULP-4·XG-100</t>
+          <t>152-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -18656,7 +18656,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>137-CO-ST-9·PVL-4·XG-100</t>
+          <t>153-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -18701,7 +18701,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>152-EC-TA-5·PRE-4·XG-100</t>
+          <t>166-EC-TA-3·ULT-4·XG-100</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -18746,7 +18746,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>153-EC-TA-5·PRE-4·XG-100</t>
+          <t>096-CH-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -18791,7 +18791,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>166-EC-TA-3·ULT-4·XG-100</t>
+          <t>555-UY-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -18836,7 +18836,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>096-CH-TA-5·PRE-4·XG-96</t>
+          <t>569-UY-TA-3·ULT-4·XG-96</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -18881,7 +18881,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>555-UY-TA-5·PRE-4·XG-96</t>
+          <t>122-CO-ST-4·ULP-3·GR-100</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -18926,7 +18926,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>569-UY-TA-3·ULT-4·XG-96</t>
+          <t>136-CO-ST-9·PVL-3·GR-100</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -18971,7 +18971,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>122-CO-ST-4·ULP-3·GR-100</t>
+          <t>148-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -19016,7 +19016,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>136-CO-ST-9·PVL-3·GR-100</t>
+          <t>149-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -19061,7 +19061,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>148-EC-TA-5·PRE-3·GR-100</t>
+          <t>163-EC-TA-3·ULT-3·GR-100</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -19106,7 +19106,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>149-EC-TA-5·PRE-3·GR-100</t>
+          <t>104-CH-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -19151,7 +19151,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>163-EC-TA-3·ULT-3·GR-100</t>
+          <t>121-CO-ST-4·ULP-2·MD-100</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -19196,7 +19196,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>104-CH-TA-5·PRE-2·MD-100</t>
+          <t>135-CO-ST-9·PVL-2·MD-100</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -19241,7 +19241,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>121-CO-ST-4·ULP-2·MD-100</t>
+          <t>144-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -19286,7 +19286,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>135-CO-ST-9·PVL-2·MD-100</t>
+          <t>145-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -19331,7 +19331,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>144-EC-TA-5·PRE-2·MD-100</t>
+          <t>160-EC-TA-3·ULT-2·MD-100</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -19376,7 +19376,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>145-EC-TA-5·PRE-2·MD-100</t>
+          <t>134-CO-TA-9·PVL-1·PQ-100</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -19421,11 +19421,11 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>160-EC-TA-3·ULT-2·MD-100</t>
+          <t>552-UY-TA-5·PRE-5·XX-96</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C134" t="n">
         <v>8.0</v>
@@ -19445,7 +19445,7 @@
         <v>0.0</v>
       </c>
       <c r="H134" t="n">
-        <v>2.8278E7</v>
+        <v>3.357E7</v>
       </c>
       <c r="I134" t="n">
         <v>0.0</v>
@@ -19466,11 +19466,11 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>134-CO-TA-9·PVL-1·PQ-100</t>
+          <t>566-UY-TA-3·ULT-5·XX-96</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C135" t="n">
         <v>8.0</v>
@@ -19490,7 +19490,7 @@
         <v>0.0</v>
       </c>
       <c r="H135" t="n">
-        <v>2.8278E7</v>
+        <v>3.357E7</v>
       </c>
       <c r="I135" t="n">
         <v>0.0</v>
@@ -19511,7 +19511,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>552-UY-TA-5·PRE-5·XX-96</t>
+          <t>123-CO-ST-4·ULP-4·XG-100</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -19556,7 +19556,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>566-UY-TA-3·ULT-5·XX-96</t>
+          <t>137-CO-ST-9·PVL-4·XG-100</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -19601,7 +19601,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>123-CO-ST-4·ULP-4·XG-100</t>
+          <t>152-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -19646,7 +19646,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>137-CO-ST-9·PVL-4·XG-100</t>
+          <t>153-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -19691,7 +19691,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>152-EC-TA-5·PRE-4·XG-100</t>
+          <t>166-EC-TA-3·ULT-4·XG-100</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -19736,7 +19736,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>153-EC-TA-5·PRE-4·XG-100</t>
+          <t>096-CH-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -19781,7 +19781,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>166-EC-TA-3·ULT-4·XG-100</t>
+          <t>555-UY-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -19826,7 +19826,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>096-CH-TA-5·PRE-4·XG-96</t>
+          <t>569-UY-TA-3·ULT-4·XG-96</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -19871,7 +19871,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>555-UY-TA-5·PRE-4·XG-96</t>
+          <t>122-CO-ST-4·ULP-3·GR-100</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -19916,7 +19916,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>569-UY-TA-3·ULT-4·XG-96</t>
+          <t>136-CO-ST-9·PVL-3·GR-100</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -19961,7 +19961,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>122-CO-ST-4·ULP-3·GR-100</t>
+          <t>148-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -20006,7 +20006,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>136-CO-ST-9·PVL-3·GR-100</t>
+          <t>149-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -20051,7 +20051,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>148-EC-TA-5·PRE-3·GR-100</t>
+          <t>163-EC-TA-3·ULT-3·GR-100</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -20096,7 +20096,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>149-EC-TA-5·PRE-3·GR-100</t>
+          <t>104-CH-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -20141,7 +20141,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>163-EC-TA-3·ULT-3·GR-100</t>
+          <t>121-CO-ST-4·ULP-2·MD-100</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -20186,7 +20186,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>104-CH-TA-5·PRE-2·MD-100</t>
+          <t>135-CO-ST-9·PVL-2·MD-100</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -20231,7 +20231,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>121-CO-ST-4·ULP-2·MD-100</t>
+          <t>144-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -20276,7 +20276,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>135-CO-ST-9·PVL-2·MD-100</t>
+          <t>145-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -20321,7 +20321,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>144-EC-TA-5·PRE-2·MD-100</t>
+          <t>160-EC-TA-3·ULT-2·MD-100</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -20366,7 +20366,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>145-EC-TA-5·PRE-2·MD-100</t>
+          <t>134-CO-TA-9·PVL-1·PQ-100</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -20411,11 +20411,11 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>160-EC-TA-3·ULT-2·MD-100</t>
+          <t>552-UY-TA-5·PRE-5·XX-96</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C156" t="n">
         <v>8.0</v>
@@ -20435,7 +20435,7 @@
         <v>0.0</v>
       </c>
       <c r="H156" t="n">
-        <v>3.357E7</v>
+        <v>3.888E7</v>
       </c>
       <c r="I156" t="n">
         <v>0.0</v>
@@ -20456,11 +20456,11 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>134-CO-TA-9·PVL-1·PQ-100</t>
+          <t>566-UY-TA-3·ULT-5·XX-96</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C157" t="n">
         <v>8.0</v>
@@ -20480,7 +20480,7 @@
         <v>0.0</v>
       </c>
       <c r="H157" t="n">
-        <v>3.357E7</v>
+        <v>3.888E7</v>
       </c>
       <c r="I157" t="n">
         <v>0.0</v>
@@ -20501,7 +20501,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>552-UY-TA-5·PRE-5·XX-96</t>
+          <t>123-CO-ST-4·ULP-4·XG-100</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -20546,7 +20546,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>566-UY-TA-3·ULT-5·XX-96</t>
+          <t>137-CO-ST-9·PVL-4·XG-100</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -20591,7 +20591,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>123-CO-ST-4·ULP-4·XG-100</t>
+          <t>152-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -20636,7 +20636,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>137-CO-ST-9·PVL-4·XG-100</t>
+          <t>153-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -20681,7 +20681,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>152-EC-TA-5·PRE-4·XG-100</t>
+          <t>166-EC-TA-3·ULT-4·XG-100</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -20726,7 +20726,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>153-EC-TA-5·PRE-4·XG-100</t>
+          <t>096-CH-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -20771,7 +20771,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>166-EC-TA-3·ULT-4·XG-100</t>
+          <t>555-UY-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -20816,7 +20816,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>096-CH-TA-5·PRE-4·XG-96</t>
+          <t>569-UY-TA-3·ULT-4·XG-96</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -20861,7 +20861,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>555-UY-TA-5·PRE-4·XG-96</t>
+          <t>122-CO-ST-4·ULP-3·GR-100</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -20906,7 +20906,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>569-UY-TA-3·ULT-4·XG-96</t>
+          <t>136-CO-ST-9·PVL-3·GR-100</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -20951,7 +20951,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>122-CO-ST-4·ULP-3·GR-100</t>
+          <t>148-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -20996,7 +20996,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>136-CO-ST-9·PVL-3·GR-100</t>
+          <t>149-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -21041,7 +21041,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>148-EC-TA-5·PRE-3·GR-100</t>
+          <t>163-EC-TA-3·ULT-3·GR-100</t>
         </is>
       </c>
       <c r="B170" t="n">
@@ -21086,7 +21086,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>149-EC-TA-5·PRE-3·GR-100</t>
+          <t>104-CH-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B171" t="n">
@@ -21131,7 +21131,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>163-EC-TA-3·ULT-3·GR-100</t>
+          <t>121-CO-ST-4·ULP-2·MD-100</t>
         </is>
       </c>
       <c r="B172" t="n">
@@ -21176,7 +21176,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>104-CH-TA-5·PRE-2·MD-100</t>
+          <t>135-CO-ST-9·PVL-2·MD-100</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -21221,7 +21221,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>121-CO-ST-4·ULP-2·MD-100</t>
+          <t>144-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -21266,7 +21266,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>135-CO-ST-9·PVL-2·MD-100</t>
+          <t>145-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -21311,7 +21311,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>144-EC-TA-5·PRE-2·MD-100</t>
+          <t>160-EC-TA-3·ULT-2·MD-100</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -21356,7 +21356,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>145-EC-TA-5·PRE-2·MD-100</t>
+          <t>134-CO-TA-9·PVL-1·PQ-100</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -21401,11 +21401,11 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>160-EC-TA-3·ULT-2·MD-100</t>
+          <t>552-UY-TA-5·PRE-5·XX-96</t>
         </is>
       </c>
       <c r="B178" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C178" t="n">
         <v>8.0</v>
@@ -21425,7 +21425,7 @@
         <v>0.0</v>
       </c>
       <c r="H178" t="n">
-        <v>3.888E7</v>
+        <v>4.4172E7</v>
       </c>
       <c r="I178" t="n">
         <v>0.0</v>
@@ -21446,11 +21446,11 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>134-CO-TA-9·PVL-1·PQ-100</t>
+          <t>566-UY-TA-3·ULT-5·XX-96</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C179" t="n">
         <v>8.0</v>
@@ -21470,7 +21470,7 @@
         <v>0.0</v>
       </c>
       <c r="H179" t="n">
-        <v>3.888E7</v>
+        <v>4.4172E7</v>
       </c>
       <c r="I179" t="n">
         <v>0.0</v>
@@ -21491,7 +21491,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>552-UY-TA-5·PRE-5·XX-96</t>
+          <t>123-CO-ST-4·ULP-4·XG-100</t>
         </is>
       </c>
       <c r="B180" t="n">
@@ -21536,7 +21536,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>566-UY-TA-3·ULT-5·XX-96</t>
+          <t>137-CO-ST-9·PVL-4·XG-100</t>
         </is>
       </c>
       <c r="B181" t="n">
@@ -21581,7 +21581,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>123-CO-ST-4·ULP-4·XG-100</t>
+          <t>152-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B182" t="n">
@@ -21626,7 +21626,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>137-CO-ST-9·PVL-4·XG-100</t>
+          <t>153-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B183" t="n">
@@ -21671,7 +21671,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>152-EC-TA-5·PRE-4·XG-100</t>
+          <t>166-EC-TA-3·ULT-4·XG-100</t>
         </is>
       </c>
       <c r="B184" t="n">
@@ -21716,7 +21716,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>153-EC-TA-5·PRE-4·XG-100</t>
+          <t>096-CH-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B185" t="n">
@@ -21761,7 +21761,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>166-EC-TA-3·ULT-4·XG-100</t>
+          <t>555-UY-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -21806,7 +21806,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>096-CH-TA-5·PRE-4·XG-96</t>
+          <t>569-UY-TA-3·ULT-4·XG-96</t>
         </is>
       </c>
       <c r="B187" t="n">
@@ -21851,7 +21851,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>555-UY-TA-5·PRE-4·XG-96</t>
+          <t>122-CO-ST-4·ULP-3·GR-100</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -21896,7 +21896,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>569-UY-TA-3·ULT-4·XG-96</t>
+          <t>136-CO-ST-9·PVL-3·GR-100</t>
         </is>
       </c>
       <c r="B189" t="n">
@@ -21941,7 +21941,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>122-CO-ST-4·ULP-3·GR-100</t>
+          <t>148-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B190" t="n">
@@ -21986,7 +21986,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>136-CO-ST-9·PVL-3·GR-100</t>
+          <t>149-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B191" t="n">
@@ -22031,7 +22031,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>148-EC-TA-5·PRE-3·GR-100</t>
+          <t>163-EC-TA-3·ULT-3·GR-100</t>
         </is>
       </c>
       <c r="B192" t="n">
@@ -22076,7 +22076,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>149-EC-TA-5·PRE-3·GR-100</t>
+          <t>104-CH-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -22121,7 +22121,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>163-EC-TA-3·ULT-3·GR-100</t>
+          <t>121-CO-ST-4·ULP-2·MD-100</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -22166,7 +22166,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>104-CH-TA-5·PRE-2·MD-100</t>
+          <t>135-CO-ST-9·PVL-2·MD-100</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -22211,7 +22211,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>121-CO-ST-4·ULP-2·MD-100</t>
+          <t>144-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -22256,7 +22256,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>135-CO-ST-9·PVL-2·MD-100</t>
+          <t>145-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B197" t="n">
@@ -22301,7 +22301,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>144-EC-TA-5·PRE-2·MD-100</t>
+          <t>160-EC-TA-3·ULT-2·MD-100</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -22346,7 +22346,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>145-EC-TA-5·PRE-2·MD-100</t>
+          <t>134-CO-TA-9·PVL-1·PQ-100</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -22391,11 +22391,11 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>160-EC-TA-3·ULT-2·MD-100</t>
+          <t>552-UY-TA-5·PRE-5·XX-96</t>
         </is>
       </c>
       <c r="B200" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="C200" t="n">
         <v>8.0</v>
@@ -22415,7 +22415,7 @@
         <v>0.0</v>
       </c>
       <c r="H200" t="n">
-        <v>4.4172E7</v>
+        <v>4.9482E7</v>
       </c>
       <c r="I200" t="n">
         <v>0.0</v>
@@ -22436,11 +22436,11 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>134-CO-TA-9·PVL-1·PQ-100</t>
+          <t>566-UY-TA-3·ULT-5·XX-96</t>
         </is>
       </c>
       <c r="B201" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="C201" t="n">
         <v>8.0</v>
@@ -22460,7 +22460,7 @@
         <v>0.0</v>
       </c>
       <c r="H201" t="n">
-        <v>4.4172E7</v>
+        <v>4.9482E7</v>
       </c>
       <c r="I201" t="n">
         <v>0.0</v>
@@ -22481,7 +22481,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>552-UY-TA-5·PRE-5·XX-96</t>
+          <t>123-CO-ST-4·ULP-4·XG-100</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -22526,7 +22526,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>566-UY-TA-3·ULT-5·XX-96</t>
+          <t>137-CO-ST-9·PVL-4·XG-100</t>
         </is>
       </c>
       <c r="B203" t="n">
@@ -22571,7 +22571,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>123-CO-ST-4·ULP-4·XG-100</t>
+          <t>152-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B204" t="n">
@@ -22616,7 +22616,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>137-CO-ST-9·PVL-4·XG-100</t>
+          <t>153-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -22661,7 +22661,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>152-EC-TA-5·PRE-4·XG-100</t>
+          <t>166-EC-TA-3·ULT-4·XG-100</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -22706,7 +22706,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>153-EC-TA-5·PRE-4·XG-100</t>
+          <t>096-CH-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -22751,7 +22751,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>166-EC-TA-3·ULT-4·XG-100</t>
+          <t>555-UY-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B208" t="n">
@@ -22796,7 +22796,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>096-CH-TA-5·PRE-4·XG-96</t>
+          <t>569-UY-TA-3·ULT-4·XG-96</t>
         </is>
       </c>
       <c r="B209" t="n">
@@ -22841,7 +22841,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>555-UY-TA-5·PRE-4·XG-96</t>
+          <t>122-CO-ST-4·ULP-3·GR-100</t>
         </is>
       </c>
       <c r="B210" t="n">
@@ -22886,7 +22886,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>569-UY-TA-3·ULT-4·XG-96</t>
+          <t>136-CO-ST-9·PVL-3·GR-100</t>
         </is>
       </c>
       <c r="B211" t="n">
@@ -22931,7 +22931,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>122-CO-ST-4·ULP-3·GR-100</t>
+          <t>148-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B212" t="n">
@@ -22976,7 +22976,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>136-CO-ST-9·PVL-3·GR-100</t>
+          <t>149-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B213" t="n">
@@ -23021,7 +23021,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>148-EC-TA-5·PRE-3·GR-100</t>
+          <t>163-EC-TA-3·ULT-3·GR-100</t>
         </is>
       </c>
       <c r="B214" t="n">
@@ -23066,7 +23066,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>149-EC-TA-5·PRE-3·GR-100</t>
+          <t>104-CH-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B215" t="n">
@@ -23111,7 +23111,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>163-EC-TA-3·ULT-3·GR-100</t>
+          <t>121-CO-ST-4·ULP-2·MD-100</t>
         </is>
       </c>
       <c r="B216" t="n">
@@ -23156,7 +23156,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>104-CH-TA-5·PRE-2·MD-100</t>
+          <t>135-CO-ST-9·PVL-2·MD-100</t>
         </is>
       </c>
       <c r="B217" t="n">
@@ -23201,7 +23201,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>121-CO-ST-4·ULP-2·MD-100</t>
+          <t>144-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B218" t="n">
@@ -23246,7 +23246,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>135-CO-ST-9·PVL-2·MD-100</t>
+          <t>145-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B219" t="n">
@@ -23291,7 +23291,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>144-EC-TA-5·PRE-2·MD-100</t>
+          <t>160-EC-TA-3·ULT-2·MD-100</t>
         </is>
       </c>
       <c r="B220" t="n">
@@ -23336,7 +23336,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>145-EC-TA-5·PRE-2·MD-100</t>
+          <t>134-CO-TA-9·PVL-1·PQ-100</t>
         </is>
       </c>
       <c r="B221" t="n">
@@ -23381,11 +23381,11 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>160-EC-TA-3·ULT-2·MD-100</t>
+          <t>552-UY-TA-5·PRE-5·XX-96</t>
         </is>
       </c>
       <c r="B222" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="C222" t="n">
         <v>8.0</v>
@@ -23405,7 +23405,7 @@
         <v>0.0</v>
       </c>
       <c r="H222" t="n">
-        <v>4.9482E7</v>
+        <v>5.4774E7</v>
       </c>
       <c r="I222" t="n">
         <v>0.0</v>
@@ -23426,11 +23426,11 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>134-CO-TA-9·PVL-1·PQ-100</t>
+          <t>566-UY-TA-3·ULT-5·XX-96</t>
         </is>
       </c>
       <c r="B223" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="C223" t="n">
         <v>8.0</v>
@@ -23450,7 +23450,7 @@
         <v>0.0</v>
       </c>
       <c r="H223" t="n">
-        <v>4.9482E7</v>
+        <v>5.4774E7</v>
       </c>
       <c r="I223" t="n">
         <v>0.0</v>
@@ -23471,7 +23471,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>552-UY-TA-5·PRE-5·XX-96</t>
+          <t>123-CO-ST-4·ULP-4·XG-100</t>
         </is>
       </c>
       <c r="B224" t="n">
@@ -23516,7 +23516,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>566-UY-TA-3·ULT-5·XX-96</t>
+          <t>137-CO-ST-9·PVL-4·XG-100</t>
         </is>
       </c>
       <c r="B225" t="n">
@@ -23561,7 +23561,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>123-CO-ST-4·ULP-4·XG-100</t>
+          <t>152-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B226" t="n">
@@ -23606,7 +23606,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>137-CO-ST-9·PVL-4·XG-100</t>
+          <t>153-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B227" t="n">
@@ -23651,7 +23651,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>152-EC-TA-5·PRE-4·XG-100</t>
+          <t>166-EC-TA-3·ULT-4·XG-100</t>
         </is>
       </c>
       <c r="B228" t="n">
@@ -23696,7 +23696,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>153-EC-TA-5·PRE-4·XG-100</t>
+          <t>096-CH-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B229" t="n">
@@ -23741,7 +23741,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>166-EC-TA-3·ULT-4·XG-100</t>
+          <t>555-UY-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B230" t="n">
@@ -23786,7 +23786,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>096-CH-TA-5·PRE-4·XG-96</t>
+          <t>569-UY-TA-3·ULT-4·XG-96</t>
         </is>
       </c>
       <c r="B231" t="n">
@@ -23831,7 +23831,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>555-UY-TA-5·PRE-4·XG-96</t>
+          <t>122-CO-ST-4·ULP-3·GR-100</t>
         </is>
       </c>
       <c r="B232" t="n">
@@ -23876,7 +23876,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>569-UY-TA-3·ULT-4·XG-96</t>
+          <t>136-CO-ST-9·PVL-3·GR-100</t>
         </is>
       </c>
       <c r="B233" t="n">
@@ -23921,7 +23921,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>122-CO-ST-4·ULP-3·GR-100</t>
+          <t>148-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B234" t="n">
@@ -23966,7 +23966,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>136-CO-ST-9·PVL-3·GR-100</t>
+          <t>149-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B235" t="n">
@@ -24011,7 +24011,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>148-EC-TA-5·PRE-3·GR-100</t>
+          <t>163-EC-TA-3·ULT-3·GR-100</t>
         </is>
       </c>
       <c r="B236" t="n">
@@ -24056,7 +24056,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>149-EC-TA-5·PRE-3·GR-100</t>
+          <t>104-CH-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B237" t="n">
@@ -24101,7 +24101,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>163-EC-TA-3·ULT-3·GR-100</t>
+          <t>121-CO-ST-4·ULP-2·MD-100</t>
         </is>
       </c>
       <c r="B238" t="n">
@@ -24146,7 +24146,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>104-CH-TA-5·PRE-2·MD-100</t>
+          <t>135-CO-ST-9·PVL-2·MD-100</t>
         </is>
       </c>
       <c r="B239" t="n">
@@ -24191,7 +24191,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>121-CO-ST-4·ULP-2·MD-100</t>
+          <t>144-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B240" t="n">
@@ -24236,7 +24236,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>135-CO-ST-9·PVL-2·MD-100</t>
+          <t>145-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B241" t="n">
@@ -24281,7 +24281,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>144-EC-TA-5·PRE-2·MD-100</t>
+          <t>160-EC-TA-3·ULT-2·MD-100</t>
         </is>
       </c>
       <c r="B242" t="n">
@@ -24326,7 +24326,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>145-EC-TA-5·PRE-2·MD-100</t>
+          <t>134-CO-TA-9·PVL-1·PQ-100</t>
         </is>
       </c>
       <c r="B243" t="n">
@@ -24371,11 +24371,11 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>160-EC-TA-3·ULT-2·MD-100</t>
+          <t>552-UY-TA-5·PRE-5·XX-96</t>
         </is>
       </c>
       <c r="B244" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="C244" t="n">
         <v>8.0</v>
@@ -24395,7 +24395,7 @@
         <v>0.0</v>
       </c>
       <c r="H244" t="n">
-        <v>5.4774E7</v>
+        <v>6.0084E7</v>
       </c>
       <c r="I244" t="n">
         <v>0.0</v>
@@ -24416,11 +24416,11 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>134-CO-TA-9·PVL-1·PQ-100</t>
+          <t>566-UY-TA-3·ULT-5·XX-96</t>
         </is>
       </c>
       <c r="B245" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="C245" t="n">
         <v>8.0</v>
@@ -24440,7 +24440,7 @@
         <v>0.0</v>
       </c>
       <c r="H245" t="n">
-        <v>5.4774E7</v>
+        <v>6.0084E7</v>
       </c>
       <c r="I245" t="n">
         <v>0.0</v>
@@ -24461,7 +24461,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>552-UY-TA-5·PRE-5·XX-96</t>
+          <t>123-CO-ST-4·ULP-4·XG-100</t>
         </is>
       </c>
       <c r="B246" t="n">
@@ -24506,7 +24506,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>566-UY-TA-3·ULT-5·XX-96</t>
+          <t>137-CO-ST-9·PVL-4·XG-100</t>
         </is>
       </c>
       <c r="B247" t="n">
@@ -24551,7 +24551,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>123-CO-ST-4·ULP-4·XG-100</t>
+          <t>152-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B248" t="n">
@@ -24596,7 +24596,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>137-CO-ST-9·PVL-4·XG-100</t>
+          <t>153-EC-TA-5·PRE-4·XG-100</t>
         </is>
       </c>
       <c r="B249" t="n">
@@ -24641,7 +24641,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>152-EC-TA-5·PRE-4·XG-100</t>
+          <t>166-EC-TA-3·ULT-4·XG-100</t>
         </is>
       </c>
       <c r="B250" t="n">
@@ -24686,7 +24686,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>153-EC-TA-5·PRE-4·XG-100</t>
+          <t>096-CH-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B251" t="n">
@@ -24731,7 +24731,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>166-EC-TA-3·ULT-4·XG-100</t>
+          <t>555-UY-TA-5·PRE-4·XG-96</t>
         </is>
       </c>
       <c r="B252" t="n">
@@ -24776,7 +24776,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>096-CH-TA-5·PRE-4·XG-96</t>
+          <t>569-UY-TA-3·ULT-4·XG-96</t>
         </is>
       </c>
       <c r="B253" t="n">
@@ -24821,7 +24821,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>555-UY-TA-5·PRE-4·XG-96</t>
+          <t>122-CO-ST-4·ULP-3·GR-100</t>
         </is>
       </c>
       <c r="B254" t="n">
@@ -24866,7 +24866,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>569-UY-TA-3·ULT-4·XG-96</t>
+          <t>136-CO-ST-9·PVL-3·GR-100</t>
         </is>
       </c>
       <c r="B255" t="n">
@@ -24911,7 +24911,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>122-CO-ST-4·ULP-3·GR-100</t>
+          <t>148-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B256" t="n">
@@ -24956,7 +24956,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>136-CO-ST-9·PVL-3·GR-100</t>
+          <t>149-EC-TA-5·PRE-3·GR-100</t>
         </is>
       </c>
       <c r="B257" t="n">
@@ -25001,7 +25001,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>148-EC-TA-5·PRE-3·GR-100</t>
+          <t>163-EC-TA-3·ULT-3·GR-100</t>
         </is>
       </c>
       <c r="B258" t="n">
@@ -25046,7 +25046,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>149-EC-TA-5·PRE-3·GR-100</t>
+          <t>104-CH-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B259" t="n">
@@ -25091,7 +25091,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>163-EC-TA-3·ULT-3·GR-100</t>
+          <t>121-CO-ST-4·ULP-2·MD-100</t>
         </is>
       </c>
       <c r="B260" t="n">
@@ -25136,7 +25136,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>104-CH-TA-5·PRE-2·MD-100</t>
+          <t>135-CO-ST-9·PVL-2·MD-100</t>
         </is>
       </c>
       <c r="B261" t="n">
@@ -25181,7 +25181,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>121-CO-ST-4·ULP-2·MD-100</t>
+          <t>144-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B262" t="n">
@@ -25226,7 +25226,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>135-CO-ST-9·PVL-2·MD-100</t>
+          <t>145-EC-TA-5·PRE-2·MD-100</t>
         </is>
       </c>
       <c r="B263" t="n">
@@ -25271,7 +25271,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>144-EC-TA-5·PRE-2·MD-100</t>
+          <t>160-EC-TA-3·ULT-2·MD-100</t>
         </is>
       </c>
       <c r="B264" t="n">
@@ -25316,7 +25316,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>145-EC-TA-5·PRE-2·MD-100</t>
+          <t>134-CO-TA-9·PVL-1·PQ-100</t>
         </is>
       </c>
       <c r="B265" t="n">
@@ -25355,1086 +25355,6 @@
         <v>0.0</v>
       </c>
       <c r="M265" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266" t="inlineStr">
-        <is>
-          <t>160-EC-TA-3·ULT-2·MD-100</t>
-        </is>
-      </c>
-      <c r="B266" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="C266" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D266" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E266" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F266" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G266" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H266" t="n">
-        <v>6.0084E7</v>
-      </c>
-      <c r="I266" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J266" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K266" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L266" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M266" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267" t="inlineStr">
-        <is>
-          <t>134-CO-TA-9·PVL-1·PQ-100</t>
-        </is>
-      </c>
-      <c r="B267" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="C267" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D267" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E267" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F267" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G267" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H267" t="n">
-        <v>6.0084E7</v>
-      </c>
-      <c r="I267" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J267" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K267" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L267" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M267" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268" t="inlineStr">
-        <is>
-          <t>552-UY-TA-5·PRE-5·XX-96</t>
-        </is>
-      </c>
-      <c r="B268" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C268" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D268" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E268" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F268" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G268" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H268" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I268" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J268" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K268" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L268" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M268" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269" t="inlineStr">
-        <is>
-          <t>566-UY-TA-3·ULT-5·XX-96</t>
-        </is>
-      </c>
-      <c r="B269" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C269" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D269" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E269" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F269" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G269" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H269" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I269" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J269" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K269" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L269" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M269" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270" t="inlineStr">
-        <is>
-          <t>123-CO-ST-4·ULP-4·XG-100</t>
-        </is>
-      </c>
-      <c r="B270" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C270" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D270" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E270" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F270" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G270" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H270" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I270" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J270" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K270" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L270" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M270" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271" t="inlineStr">
-        <is>
-          <t>137-CO-ST-9·PVL-4·XG-100</t>
-        </is>
-      </c>
-      <c r="B271" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C271" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D271" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E271" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F271" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G271" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H271" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I271" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J271" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K271" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L271" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M271" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="272">
-      <c r="A272" t="inlineStr">
-        <is>
-          <t>152-EC-TA-5·PRE-4·XG-100</t>
-        </is>
-      </c>
-      <c r="B272" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C272" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D272" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E272" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F272" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G272" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H272" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I272" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J272" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K272" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L272" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M272" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273" t="inlineStr">
-        <is>
-          <t>153-EC-TA-5·PRE-4·XG-100</t>
-        </is>
-      </c>
-      <c r="B273" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C273" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D273" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E273" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F273" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G273" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H273" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I273" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J273" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K273" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L273" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M273" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274" t="inlineStr">
-        <is>
-          <t>166-EC-TA-3·ULT-4·XG-100</t>
-        </is>
-      </c>
-      <c r="B274" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C274" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D274" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E274" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F274" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G274" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H274" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I274" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J274" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K274" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L274" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M274" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275" t="inlineStr">
-        <is>
-          <t>096-CH-TA-5·PRE-4·XG-96</t>
-        </is>
-      </c>
-      <c r="B275" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C275" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D275" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E275" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F275" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G275" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H275" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I275" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J275" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K275" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L275" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M275" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="276">
-      <c r="A276" t="inlineStr">
-        <is>
-          <t>555-UY-TA-5·PRE-4·XG-96</t>
-        </is>
-      </c>
-      <c r="B276" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C276" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D276" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E276" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F276" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G276" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H276" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I276" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J276" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K276" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L276" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M276" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="277">
-      <c r="A277" t="inlineStr">
-        <is>
-          <t>569-UY-TA-3·ULT-4·XG-96</t>
-        </is>
-      </c>
-      <c r="B277" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C277" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D277" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E277" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F277" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G277" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H277" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I277" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J277" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K277" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L277" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M277" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="278">
-      <c r="A278" t="inlineStr">
-        <is>
-          <t>122-CO-ST-4·ULP-3·GR-100</t>
-        </is>
-      </c>
-      <c r="B278" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C278" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D278" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E278" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F278" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G278" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H278" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I278" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J278" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K278" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L278" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M278" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="279">
-      <c r="A279" t="inlineStr">
-        <is>
-          <t>136-CO-ST-9·PVL-3·GR-100</t>
-        </is>
-      </c>
-      <c r="B279" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C279" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D279" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E279" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F279" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G279" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H279" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I279" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J279" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K279" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L279" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M279" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="280">
-      <c r="A280" t="inlineStr">
-        <is>
-          <t>148-EC-TA-5·PRE-3·GR-100</t>
-        </is>
-      </c>
-      <c r="B280" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C280" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D280" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E280" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F280" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G280" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H280" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I280" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J280" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K280" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L280" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M280" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="281">
-      <c r="A281" t="inlineStr">
-        <is>
-          <t>149-EC-TA-5·PRE-3·GR-100</t>
-        </is>
-      </c>
-      <c r="B281" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C281" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D281" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E281" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F281" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G281" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H281" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I281" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J281" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K281" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L281" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M281" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="282">
-      <c r="A282" t="inlineStr">
-        <is>
-          <t>163-EC-TA-3·ULT-3·GR-100</t>
-        </is>
-      </c>
-      <c r="B282" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C282" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D282" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E282" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F282" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G282" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H282" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I282" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J282" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K282" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L282" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M282" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="283">
-      <c r="A283" t="inlineStr">
-        <is>
-          <t>104-CH-TA-5·PRE-2·MD-100</t>
-        </is>
-      </c>
-      <c r="B283" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C283" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D283" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E283" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F283" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G283" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H283" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I283" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J283" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K283" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L283" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M283" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="A284" t="inlineStr">
-        <is>
-          <t>121-CO-ST-4·ULP-2·MD-100</t>
-        </is>
-      </c>
-      <c r="B284" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C284" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D284" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E284" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F284" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G284" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H284" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I284" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J284" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K284" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L284" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M284" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="285">
-      <c r="A285" t="inlineStr">
-        <is>
-          <t>135-CO-ST-9·PVL-2·MD-100</t>
-        </is>
-      </c>
-      <c r="B285" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C285" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D285" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E285" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F285" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G285" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H285" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I285" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J285" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K285" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L285" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M285" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286" t="inlineStr">
-        <is>
-          <t>144-EC-TA-5·PRE-2·MD-100</t>
-        </is>
-      </c>
-      <c r="B286" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C286" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D286" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E286" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F286" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G286" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H286" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I286" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J286" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K286" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L286" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M286" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="287">
-      <c r="A287" t="inlineStr">
-        <is>
-          <t>145-EC-TA-5·PRE-2·MD-100</t>
-        </is>
-      </c>
-      <c r="B287" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C287" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D287" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E287" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F287" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G287" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H287" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I287" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J287" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K287" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L287" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M287" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="288">
-      <c r="A288" t="inlineStr">
-        <is>
-          <t>160-EC-TA-3·ULT-2·MD-100</t>
-        </is>
-      </c>
-      <c r="B288" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C288" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D288" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E288" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F288" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G288" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H288" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I288" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J288" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K288" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L288" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M288" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="289">
-      <c r="A289" t="inlineStr">
-        <is>
-          <t>134-CO-TA-9·PVL-1·PQ-100</t>
-        </is>
-      </c>
-      <c r="B289" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C289" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D289" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E289" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F289" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G289" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H289" t="n">
-        <v>6.5376E7</v>
-      </c>
-      <c r="I289" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J289" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K289" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L289" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="M289" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -28512,190 +27432,6 @@
         <v>10800.0</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B90" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C90" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D90" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E90" t="n">
-        <v>3110400.0</v>
-      </c>
-      <c r="F90" t="n">
-        <v>3877.3202793598866</v>
-      </c>
-      <c r="G90" t="n">
-        <v>54000.0</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B91" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C91" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D91" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E91" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F91" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G91" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B92" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C92" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D92" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E92" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F92" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G92" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B93" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C93" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D93" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E93" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F93" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G93" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B94" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C94" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D94" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E94" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F94" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G94" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="B95" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C95" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D95" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E95" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F95" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G95" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="B96" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C96" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D96" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E96" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F96" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G96" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="B97" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C97" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D97" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E97" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F97" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G97" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -28907,22 +27643,6 @@
         <v>129716.65854594347</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>091-CH-TA-5·PRE-5·XX-96</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1.05408E7</v>
-      </c>
-      <c r="D13" t="n">
-        <v>136426.5445534472</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambios en la linea de produccion para CO correctos
</commit_message>
<xml_diff>
--- a/CMPC_Manufacturing/OutputCMPC.xlsx
+++ b/CMPC_Manufacturing/OutputCMPC.xlsx
@@ -166,7 +166,7 @@
         <v>2.0</v>
       </c>
       <c r="E2" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F2" t="n">
         <v>2.0</v>
@@ -178,7 +178,7 @@
         <v>10672.48</v>
       </c>
       <c r="I2" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J2" t="n">
         <v>2912.0</v>
@@ -190,10 +190,10 @@
         <v>1.3986E7</v>
       </c>
       <c r="M2" t="n">
-        <v>47516.733101538455</v>
+        <v>47190.818906153836</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
     </row>
     <row r="3">
@@ -212,7 +212,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F3" t="n">
         <v>2.0</v>
@@ -224,7 +224,7 @@
         <v>10672.48</v>
       </c>
       <c r="I3" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J3" t="n">
         <v>2912.0</v>
@@ -236,10 +236,10 @@
         <v>1.3986E7</v>
       </c>
       <c r="M3" t="n">
-        <v>47516.733101538455</v>
+        <v>47190.818906153836</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
     </row>
     <row r="4">
@@ -258,7 +258,7 @@
         <v>2.0</v>
       </c>
       <c r="E4" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F4" t="n">
         <v>2.0</v>
@@ -270,7 +270,7 @@
         <v>10672.48</v>
       </c>
       <c r="I4" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J4" t="n">
         <v>2912.0</v>
@@ -282,10 +282,10 @@
         <v>1.3986E7</v>
       </c>
       <c r="M4" t="n">
-        <v>47516.733101538455</v>
+        <v>47190.818906153836</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
     </row>
     <row r="5">
@@ -304,7 +304,7 @@
         <v>2.0</v>
       </c>
       <c r="E5" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F5" t="n">
         <v>2.0</v>
@@ -316,7 +316,7 @@
         <v>10672.48</v>
       </c>
       <c r="I5" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J5" t="n">
         <v>2912.0</v>
@@ -328,10 +328,10 @@
         <v>1.3986E7</v>
       </c>
       <c r="M5" t="n">
-        <v>47516.733101538455</v>
+        <v>47190.818906153836</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
     </row>
     <row r="6">
@@ -350,7 +350,7 @@
         <v>2.0</v>
       </c>
       <c r="E6" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F6" t="n">
         <v>2.0</v>
@@ -362,7 +362,7 @@
         <v>10672.48</v>
       </c>
       <c r="I6" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J6" t="n">
         <v>2912.0</v>
@@ -374,10 +374,10 @@
         <v>1.3986E7</v>
       </c>
       <c r="M6" t="n">
-        <v>47516.733101538455</v>
+        <v>47190.818906153836</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
     </row>
     <row r="7">
@@ -396,7 +396,7 @@
         <v>2.0</v>
       </c>
       <c r="E7" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F7" t="n">
         <v>2.0</v>
@@ -408,7 +408,7 @@
         <v>10672.48</v>
       </c>
       <c r="I7" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J7" t="n">
         <v>2912.0</v>
@@ -420,10 +420,10 @@
         <v>1.3986E7</v>
       </c>
       <c r="M7" t="n">
-        <v>47516.733101538455</v>
+        <v>47190.818906153836</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
     </row>
     <row r="8">
@@ -442,7 +442,7 @@
         <v>2.0</v>
       </c>
       <c r="E8" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F8" t="n">
         <v>2.0</v>
@@ -454,7 +454,7 @@
         <v>10672.48</v>
       </c>
       <c r="I8" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J8" t="n">
         <v>2912.0</v>
@@ -466,10 +466,10 @@
         <v>1.3986E7</v>
       </c>
       <c r="M8" t="n">
-        <v>47516.733101538455</v>
+        <v>47190.818906153836</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
     </row>
     <row r="9">
@@ -488,7 +488,7 @@
         <v>2.0</v>
       </c>
       <c r="E9" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F9" t="n">
         <v>2.0</v>
@@ -500,7 +500,7 @@
         <v>10672.48</v>
       </c>
       <c r="I9" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J9" t="n">
         <v>2912.0</v>
@@ -512,10 +512,10 @@
         <v>1.3986E7</v>
       </c>
       <c r="M9" t="n">
-        <v>47516.733101538455</v>
+        <v>47190.818906153836</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
     </row>
     <row r="10">
@@ -534,7 +534,7 @@
         <v>2.0</v>
       </c>
       <c r="E10" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F10" t="n">
         <v>2.0</v>
@@ -546,7 +546,7 @@
         <v>10672.48</v>
       </c>
       <c r="I10" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J10" t="n">
         <v>2912.0</v>
@@ -558,10 +558,10 @@
         <v>1.3986E7</v>
       </c>
       <c r="M10" t="n">
-        <v>47516.733101538455</v>
+        <v>47190.818906153836</v>
       </c>
       <c r="N10" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
     </row>
     <row r="11">
@@ -580,7 +580,7 @@
         <v>2.0</v>
       </c>
       <c r="E11" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F11" t="n">
         <v>2.0</v>
@@ -592,7 +592,7 @@
         <v>10672.48</v>
       </c>
       <c r="I11" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J11" t="n">
         <v>2912.0</v>
@@ -604,10 +604,10 @@
         <v>1.3986E7</v>
       </c>
       <c r="M11" t="n">
-        <v>47516.733101538455</v>
+        <v>47190.818906153836</v>
       </c>
       <c r="N11" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
     </row>
     <row r="12">
@@ -626,7 +626,7 @@
         <v>2.0</v>
       </c>
       <c r="E12" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F12" t="n">
         <v>2.0</v>
@@ -638,7 +638,7 @@
         <v>10672.48</v>
       </c>
       <c r="I12" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J12" t="n">
         <v>2912.0</v>
@@ -650,10 +650,10 @@
         <v>1.3986E7</v>
       </c>
       <c r="M12" t="n">
-        <v>47516.733101538455</v>
+        <v>47190.818906153836</v>
       </c>
       <c r="N12" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
     </row>
     <row r="13">
@@ -672,7 +672,7 @@
         <v>2.0</v>
       </c>
       <c r="E13" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F13" t="n">
         <v>2.0</v>
@@ -684,7 +684,7 @@
         <v>10672.48</v>
       </c>
       <c r="I13" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J13" t="n">
         <v>2912.0</v>
@@ -696,10 +696,10 @@
         <v>1.3986E7</v>
       </c>
       <c r="M13" t="n">
-        <v>47516.733101538455</v>
+        <v>47190.818906153836</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
     </row>
     <row r="14">
@@ -718,7 +718,7 @@
         <v>2.0</v>
       </c>
       <c r="E14" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F14" t="n">
         <v>3.0</v>
@@ -730,7 +730,7 @@
         <v>16008.719999999998</v>
       </c>
       <c r="I14" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J14" t="n">
         <v>3000.0</v>
@@ -742,10 +742,10 @@
         <v>1.4148E7</v>
       </c>
       <c r="M14" t="n">
-        <v>63850.27126153845</v>
+        <v>63524.35706615383</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0045130245449207275</v>
+        <v>0.004489988483612796</v>
       </c>
     </row>
     <row r="15">
@@ -764,7 +764,7 @@
         <v>2.0</v>
       </c>
       <c r="E15" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F15" t="n">
         <v>3.0</v>
@@ -776,7 +776,7 @@
         <v>16008.719999999998</v>
       </c>
       <c r="I15" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J15" t="n">
         <v>3000.0</v>
@@ -788,10 +788,10 @@
         <v>1.7676E7</v>
       </c>
       <c r="M15" t="n">
-        <v>63850.27126153845</v>
+        <v>63524.35706615383</v>
       </c>
       <c r="N15" t="n">
-        <v>0.0036122579351402155</v>
+        <v>0.0035938197027695087</v>
       </c>
     </row>
     <row r="16">
@@ -810,7 +810,7 @@
         <v>2.0</v>
       </c>
       <c r="E16" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F16" t="n">
         <v>3.0</v>
@@ -822,7 +822,7 @@
         <v>16008.719999999998</v>
       </c>
       <c r="I16" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J16" t="n">
         <v>3000.0</v>
@@ -834,10 +834,10 @@
         <v>1.944E7</v>
       </c>
       <c r="M16" t="n">
-        <v>63850.27126153845</v>
+        <v>63524.35706615383</v>
       </c>
       <c r="N16" t="n">
-        <v>0.0032844789743589737</v>
+        <v>0.0032677138408515344</v>
       </c>
     </row>
     <row r="17">
@@ -856,7 +856,7 @@
         <v>2.0</v>
       </c>
       <c r="E17" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F17" t="n">
         <v>3.0</v>
@@ -868,7 +868,7 @@
         <v>16008.719999999998</v>
       </c>
       <c r="I17" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J17" t="n">
         <v>3000.0</v>
@@ -880,10 +880,10 @@
         <v>2.0304E7</v>
       </c>
       <c r="M17" t="n">
-        <v>63850.27126153845</v>
+        <v>63524.35706615383</v>
       </c>
       <c r="N17" t="n">
-        <v>0.003144713911620294</v>
+        <v>0.0031286621880493417</v>
       </c>
     </row>
     <row r="18">
@@ -902,7 +902,7 @@
         <v>2.0</v>
       </c>
       <c r="E18" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F18" t="n">
         <v>3.0</v>
@@ -914,7 +914,7 @@
         <v>16008.719999999998</v>
       </c>
       <c r="I18" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J18" t="n">
         <v>3000.0</v>
@@ -926,10 +926,10 @@
         <v>2.0772E7</v>
       </c>
       <c r="M18" t="n">
-        <v>63850.27126153845</v>
+        <v>63524.35706615383</v>
       </c>
       <c r="N18" t="n">
-        <v>0.0030738624716704433</v>
+        <v>0.0030581723987172073</v>
       </c>
     </row>
     <row r="19">
@@ -948,7 +948,7 @@
         <v>2.0</v>
       </c>
       <c r="E19" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F19" t="n">
         <v>3.0</v>
@@ -960,7 +960,7 @@
         <v>16008.719999999998</v>
       </c>
       <c r="I19" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J19" t="n">
         <v>3000.0</v>
@@ -972,10 +972,10 @@
         <v>2.0988E7</v>
       </c>
       <c r="M19" t="n">
-        <v>63850.27126153845</v>
+        <v>63524.35706615383</v>
       </c>
       <c r="N19" t="n">
-        <v>0.003042227523419976</v>
+        <v>0.00302669892634619</v>
       </c>
     </row>
     <row r="20">
@@ -994,7 +994,7 @@
         <v>2.0</v>
       </c>
       <c r="E20" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F20" t="n">
         <v>3.0</v>
@@ -1006,7 +1006,7 @@
         <v>16008.719999999998</v>
       </c>
       <c r="I20" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J20" t="n">
         <v>3000.0</v>
@@ -1018,10 +1018,10 @@
         <v>2.1096E7</v>
       </c>
       <c r="M20" t="n">
-        <v>63850.27126153845</v>
+        <v>63524.35706615383</v>
       </c>
       <c r="N20" t="n">
-        <v>0.00302665297978472</v>
+        <v>0.0030112038806481716</v>
       </c>
     </row>
     <row r="21">
@@ -1040,7 +1040,7 @@
         <v>2.0</v>
       </c>
       <c r="E21" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F21" t="n">
         <v>3.0</v>
@@ -1052,7 +1052,7 @@
         <v>16008.719999999998</v>
       </c>
       <c r="I21" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J21" t="n">
         <v>3000.0</v>
@@ -1064,10 +1064,10 @@
         <v>2.1114E7</v>
       </c>
       <c r="M21" t="n">
-        <v>63850.27126153845</v>
+        <v>63524.35706615383</v>
       </c>
       <c r="N21" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
     </row>
     <row r="22">
@@ -1086,7 +1086,7 @@
         <v>2.0</v>
       </c>
       <c r="E22" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F22" t="n">
         <v>3.0</v>
@@ -1098,7 +1098,7 @@
         <v>16008.719999999998</v>
       </c>
       <c r="I22" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J22" t="n">
         <v>3000.0</v>
@@ -1110,10 +1110,10 @@
         <v>2.1114E7</v>
       </c>
       <c r="M22" t="n">
-        <v>63850.27126153845</v>
+        <v>63524.35706615383</v>
       </c>
       <c r="N22" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
     </row>
     <row r="23">
@@ -1132,7 +1132,7 @@
         <v>2.0</v>
       </c>
       <c r="E23" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F23" t="n">
         <v>3.0</v>
@@ -1144,7 +1144,7 @@
         <v>16008.719999999998</v>
       </c>
       <c r="I23" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J23" t="n">
         <v>3000.0</v>
@@ -1156,10 +1156,10 @@
         <v>2.1114E7</v>
       </c>
       <c r="M23" t="n">
-        <v>63850.27126153845</v>
+        <v>63524.35706615383</v>
       </c>
       <c r="N23" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
     </row>
     <row r="24">
@@ -1178,7 +1178,7 @@
         <v>2.0</v>
       </c>
       <c r="E24" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F24" t="n">
         <v>3.0</v>
@@ -1190,7 +1190,7 @@
         <v>16008.719999999998</v>
       </c>
       <c r="I24" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J24" t="n">
         <v>3000.0</v>
@@ -1202,10 +1202,10 @@
         <v>2.1114E7</v>
       </c>
       <c r="M24" t="n">
-        <v>63850.27126153845</v>
+        <v>63524.35706615383</v>
       </c>
       <c r="N24" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
     </row>
     <row r="25">
@@ -1224,7 +1224,7 @@
         <v>2.0</v>
       </c>
       <c r="E25" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="F25" t="n">
         <v>3.0</v>
@@ -1236,7 +1236,7 @@
         <v>16008.719999999998</v>
       </c>
       <c r="I25" t="n">
-        <v>1303.6567815384612</v>
+        <v>977.7425861538459</v>
       </c>
       <c r="J25" t="n">
         <v>3000.0</v>
@@ -1248,10 +1248,10 @@
         <v>2.1114E7</v>
       </c>
       <c r="M25" t="n">
-        <v>63850.27126153845</v>
+        <v>63524.35706615383</v>
       </c>
       <c r="N25" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
     </row>
     <row r="26">
@@ -1270,7 +1270,7 @@
         <v>1.0</v>
       </c>
       <c r="E26" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="F26" t="n">
         <v>1.0</v>
@@ -1282,7 +1282,7 @@
         <v>5336.24</v>
       </c>
       <c r="I26" t="n">
-        <v>602.2074584615383</v>
+        <v>451.6555938461537</v>
       </c>
       <c r="J26" t="n">
         <v>3760.0</v>
@@ -1294,10 +1294,10 @@
         <v>2664000.0</v>
       </c>
       <c r="M26" t="n">
-        <v>29547.601378461535</v>
+        <v>29397.04951384615</v>
       </c>
       <c r="N26" t="n">
-        <v>0.011091441958881957</v>
+        <v>0.011034928496188494</v>
       </c>
     </row>
     <row r="27">
@@ -13508,7 +13508,7 @@
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>215.5704225352124</v>
+        <v>213.57042253521237</v>
       </c>
       <c r="J2" t="n">
         <v>207.57042253521232</v>
@@ -13517,10 +13517,10 @@
         <v>0.10227442708333333</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M2" t="n">
-        <v>0.10567187689754313</v>
+        <v>0.10564857400927025</v>
       </c>
     </row>
     <row r="3">
@@ -13553,7 +13553,7 @@
         <v>0.0</v>
       </c>
       <c r="I3" t="n">
-        <v>210.8169014084518</v>
+        <v>208.81690140845177</v>
       </c>
       <c r="J3" t="n">
         <v>202.8169014084517</v>
@@ -13562,10 +13562,10 @@
         <v>0.0673465148754811</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M3" t="n">
-        <v>0.07074396468969091</v>
+        <v>0.07072066180141802</v>
       </c>
     </row>
     <row r="4">
@@ -13598,7 +13598,7 @@
         <v>0.0</v>
       </c>
       <c r="I4" t="n">
-        <v>215.5704225352124</v>
+        <v>213.57042253521237</v>
       </c>
       <c r="J4" t="n">
         <v>207.57042253521232</v>
@@ -13607,10 +13607,10 @@
         <v>0.11347199999999998</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0045130245449207275</v>
+        <v>0.004489988483612796</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1179850245449207</v>
+        <v>0.11796198848361278</v>
       </c>
     </row>
     <row r="5">
@@ -13643,7 +13643,7 @@
         <v>0.0</v>
       </c>
       <c r="I5" t="n">
-        <v>215.5704225352124</v>
+        <v>213.57042253521237</v>
       </c>
       <c r="J5" t="n">
         <v>207.57042253521232</v>
@@ -13652,10 +13652,10 @@
         <v>0.061613305263157885</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0045130245449207275</v>
+        <v>0.004489988483612796</v>
       </c>
       <c r="M5" t="n">
-        <v>0.06612632980807862</v>
+        <v>0.06610329374677068</v>
       </c>
     </row>
     <row r="6">
@@ -13688,7 +13688,7 @@
         <v>0.0</v>
       </c>
       <c r="I6" t="n">
-        <v>216.45070422535133</v>
+        <v>214.45070422535136</v>
       </c>
       <c r="J6" t="n">
         <v>208.4507042253514</v>
@@ -13697,10 +13697,10 @@
         <v>0.08422561052631579</v>
       </c>
       <c r="L6" t="n">
-        <v>0.011091441958881957</v>
+        <v>0.011034928496188494</v>
       </c>
       <c r="M6" t="n">
-        <v>0.09531705248519774</v>
+        <v>0.09526053902250428</v>
       </c>
     </row>
     <row r="7">
@@ -13733,7 +13733,7 @@
         <v>0.0</v>
       </c>
       <c r="I7" t="n">
-        <v>267.3309859154939</v>
+        <v>265.330985915494</v>
       </c>
       <c r="J7" t="n">
         <v>259.33098591549424</v>
@@ -13742,10 +13742,10 @@
         <v>0.10227442708333333</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M7" t="n">
-        <v>0.10567187689754313</v>
+        <v>0.10564857400927025</v>
       </c>
     </row>
     <row r="8">
@@ -13778,7 +13778,7 @@
         <v>0.0</v>
       </c>
       <c r="I8" t="n">
-        <v>159.05633802816968</v>
+        <v>157.05633802816965</v>
       </c>
       <c r="J8" t="n">
         <v>151.0563380281696</v>
@@ -13787,10 +13787,10 @@
         <v>0.0673465148754811</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M8" t="n">
-        <v>0.07074396468969091</v>
+        <v>0.07072066180141802</v>
       </c>
     </row>
     <row r="9">
@@ -13823,7 +13823,7 @@
         <v>0.0</v>
       </c>
       <c r="I9" t="n">
-        <v>267.3309859154939</v>
+        <v>265.330985915494</v>
       </c>
       <c r="J9" t="n">
         <v>259.33098591549424</v>
@@ -13832,10 +13832,10 @@
         <v>0.11347199999999998</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0036122579351402155</v>
+        <v>0.0035938197027695087</v>
       </c>
       <c r="M9" t="n">
-        <v>0.11708425793514018</v>
+        <v>0.11706581970276948</v>
       </c>
     </row>
     <row r="10">
@@ -13868,7 +13868,7 @@
         <v>0.0</v>
       </c>
       <c r="I10" t="n">
-        <v>267.3309859154939</v>
+        <v>265.330985915494</v>
       </c>
       <c r="J10" t="n">
         <v>259.33098591549424</v>
@@ -13877,10 +13877,10 @@
         <v>0.061613305263157885</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0036122579351402155</v>
+        <v>0.0035938197027695087</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0652255631982981</v>
+        <v>0.0652071249659274</v>
       </c>
     </row>
     <row r="11">
@@ -13958,7 +13958,7 @@
         <v>0.0</v>
       </c>
       <c r="I12" t="n">
-        <v>293.21126760563357</v>
+        <v>291.2112676056337</v>
       </c>
       <c r="J12" t="n">
         <v>285.2112676056339</v>
@@ -13967,10 +13967,10 @@
         <v>0.10227442708333333</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M12" t="n">
-        <v>0.10567187689754313</v>
+        <v>0.10564857400927025</v>
       </c>
     </row>
     <row r="13">
@@ -14003,7 +14003,7 @@
         <v>0.0</v>
       </c>
       <c r="I13" t="n">
-        <v>133.17605633802862</v>
+        <v>131.1760563380286</v>
       </c>
       <c r="J13" t="n">
         <v>125.17605633802854</v>
@@ -14012,10 +14012,10 @@
         <v>0.0673465148754811</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M13" t="n">
-        <v>0.07074396468969091</v>
+        <v>0.07072066180141802</v>
       </c>
     </row>
     <row r="14">
@@ -14048,7 +14048,7 @@
         <v>0.0</v>
       </c>
       <c r="I14" t="n">
-        <v>293.21126760563357</v>
+        <v>291.2112676056337</v>
       </c>
       <c r="J14" t="n">
         <v>285.2112676056339</v>
@@ -14057,10 +14057,10 @@
         <v>0.11347199999999998</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0032844789743589737</v>
+        <v>0.0032677138408515344</v>
       </c>
       <c r="M14" t="n">
-        <v>0.11675647897435895</v>
+        <v>0.11673971384085151</v>
       </c>
     </row>
     <row r="15">
@@ -14093,7 +14093,7 @@
         <v>0.0</v>
       </c>
       <c r="I15" t="n">
-        <v>293.21126760563357</v>
+        <v>291.2112676056337</v>
       </c>
       <c r="J15" t="n">
         <v>285.2112676056339</v>
@@ -14102,10 +14102,10 @@
         <v>0.061613305263157885</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0032844789743589737</v>
+        <v>0.0032677138408515344</v>
       </c>
       <c r="M15" t="n">
-        <v>0.06489778423751685</v>
+        <v>0.06488101910400942</v>
       </c>
     </row>
     <row r="16">
@@ -14183,7 +14183,7 @@
         <v>0.0</v>
       </c>
       <c r="I17" t="n">
-        <v>305.88732394366116</v>
+        <v>303.8873239436613</v>
       </c>
       <c r="J17" t="n">
         <v>297.8873239436615</v>
@@ -14192,10 +14192,10 @@
         <v>0.10227442708333333</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M17" t="n">
-        <v>0.10567187689754313</v>
+        <v>0.10564857400927025</v>
       </c>
     </row>
     <row r="18">
@@ -14228,7 +14228,7 @@
         <v>0.0</v>
       </c>
       <c r="I18" t="n">
-        <v>120.50000000000034</v>
+        <v>118.50000000000033</v>
       </c>
       <c r="J18" t="n">
         <v>112.50000000000027</v>
@@ -14237,10 +14237,10 @@
         <v>0.0673465148754811</v>
       </c>
       <c r="L18" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M18" t="n">
-        <v>0.07074396468969091</v>
+        <v>0.07072066180141802</v>
       </c>
     </row>
     <row r="19">
@@ -14273,7 +14273,7 @@
         <v>0.0</v>
       </c>
       <c r="I19" t="n">
-        <v>305.88732394366116</v>
+        <v>303.8873239436613</v>
       </c>
       <c r="J19" t="n">
         <v>297.8873239436615</v>
@@ -14282,10 +14282,10 @@
         <v>0.11347199999999998</v>
       </c>
       <c r="L19" t="n">
-        <v>0.003144713911620294</v>
+        <v>0.0031286621880493417</v>
       </c>
       <c r="M19" t="n">
-        <v>0.11661671391162028</v>
+        <v>0.11660066218804932</v>
       </c>
     </row>
     <row r="20">
@@ -14318,7 +14318,7 @@
         <v>0.0</v>
       </c>
       <c r="I20" t="n">
-        <v>305.88732394366116</v>
+        <v>303.8873239436613</v>
       </c>
       <c r="J20" t="n">
         <v>297.8873239436615</v>
@@ -14327,10 +14327,10 @@
         <v>0.061613305263157885</v>
       </c>
       <c r="L20" t="n">
-        <v>0.003144713911620294</v>
+        <v>0.0031286621880493417</v>
       </c>
       <c r="M20" t="n">
-        <v>0.06475801917477818</v>
+        <v>0.06474196745120722</v>
       </c>
     </row>
     <row r="21">
@@ -14408,7 +14408,7 @@
         <v>0.0</v>
       </c>
       <c r="I22" t="n">
-        <v>312.75352112675944</v>
+        <v>310.75352112675955</v>
       </c>
       <c r="J22" t="n">
         <v>304.7535211267598</v>
@@ -14417,10 +14417,10 @@
         <v>0.10227442708333333</v>
       </c>
       <c r="L22" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M22" t="n">
-        <v>0.10567187689754313</v>
+        <v>0.10564857400927025</v>
       </c>
     </row>
     <row r="23">
@@ -14453,7 +14453,7 @@
         <v>0.0</v>
       </c>
       <c r="I23" t="n">
-        <v>113.63380281690169</v>
+        <v>111.63380281690168</v>
       </c>
       <c r="J23" t="n">
         <v>105.63380281690162</v>
@@ -14462,10 +14462,10 @@
         <v>0.0673465148754811</v>
       </c>
       <c r="L23" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M23" t="n">
-        <v>0.07074396468969091</v>
+        <v>0.07072066180141802</v>
       </c>
     </row>
     <row r="24">
@@ -14498,7 +14498,7 @@
         <v>0.0</v>
       </c>
       <c r="I24" t="n">
-        <v>312.75352112675944</v>
+        <v>310.75352112675955</v>
       </c>
       <c r="J24" t="n">
         <v>304.7535211267598</v>
@@ -14507,10 +14507,10 @@
         <v>0.11347199999999998</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0030738624716704433</v>
+        <v>0.0030581723987172073</v>
       </c>
       <c r="M24" t="n">
-        <v>0.11654586247167043</v>
+        <v>0.11653017239871719</v>
       </c>
     </row>
     <row r="25">
@@ -14543,7 +14543,7 @@
         <v>0.0</v>
       </c>
       <c r="I25" t="n">
-        <v>312.75352112675944</v>
+        <v>310.75352112675955</v>
       </c>
       <c r="J25" t="n">
         <v>304.7535211267598</v>
@@ -14552,10 +14552,10 @@
         <v>0.061613305263157885</v>
       </c>
       <c r="L25" t="n">
-        <v>0.0030738624716704433</v>
+        <v>0.0030581723987172073</v>
       </c>
       <c r="M25" t="n">
-        <v>0.06468716773482833</v>
+        <v>0.06467147766187509</v>
       </c>
     </row>
     <row r="26">
@@ -14633,7 +14633,7 @@
         <v>0.0</v>
       </c>
       <c r="I27" t="n">
-        <v>315.92253521126634</v>
+        <v>313.92253521126645</v>
       </c>
       <c r="J27" t="n">
         <v>307.9225352112667</v>
@@ -14642,10 +14642,10 @@
         <v>0.10227442708333333</v>
       </c>
       <c r="L27" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M27" t="n">
-        <v>0.10567187689754313</v>
+        <v>0.10564857400927025</v>
       </c>
     </row>
     <row r="28">
@@ -14678,7 +14678,7 @@
         <v>0.0</v>
       </c>
       <c r="I28" t="n">
-        <v>110.46478873239462</v>
+        <v>108.46478873239461</v>
       </c>
       <c r="J28" t="n">
         <v>102.46478873239455</v>
@@ -14687,10 +14687,10 @@
         <v>0.0673465148754811</v>
       </c>
       <c r="L28" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M28" t="n">
-        <v>0.07074396468969091</v>
+        <v>0.07072066180141802</v>
       </c>
     </row>
     <row r="29">
@@ -14723,7 +14723,7 @@
         <v>0.0</v>
       </c>
       <c r="I29" t="n">
-        <v>315.92253521126634</v>
+        <v>313.92253521126645</v>
       </c>
       <c r="J29" t="n">
         <v>307.9225352112667</v>
@@ -14732,10 +14732,10 @@
         <v>0.11347199999999998</v>
       </c>
       <c r="L29" t="n">
-        <v>0.003042227523419976</v>
+        <v>0.00302669892634619</v>
       </c>
       <c r="M29" t="n">
-        <v>0.11651422752341996</v>
+        <v>0.11649869892634616</v>
       </c>
     </row>
     <row r="30">
@@ -14768,7 +14768,7 @@
         <v>0.0</v>
       </c>
       <c r="I30" t="n">
-        <v>315.92253521126634</v>
+        <v>313.92253521126645</v>
       </c>
       <c r="J30" t="n">
         <v>307.9225352112667</v>
@@ -14777,10 +14777,10 @@
         <v>0.061613305263157885</v>
       </c>
       <c r="L30" t="n">
-        <v>0.003042227523419976</v>
+        <v>0.00302669892634619</v>
       </c>
       <c r="M30" t="n">
-        <v>0.06465553278657786</v>
+        <v>0.06464000418950408</v>
       </c>
     </row>
     <row r="31">
@@ -14858,7 +14858,7 @@
         <v>0.0</v>
       </c>
       <c r="I32" t="n">
-        <v>317.5070422535198</v>
+        <v>315.5070422535199</v>
       </c>
       <c r="J32" t="n">
         <v>309.5070422535201</v>
@@ -14867,10 +14867,10 @@
         <v>0.10227442708333333</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M32" t="n">
-        <v>0.10567187689754313</v>
+        <v>0.10564857400927025</v>
       </c>
     </row>
     <row r="33">
@@ -14903,7 +14903,7 @@
         <v>0.0</v>
       </c>
       <c r="I33" t="n">
-        <v>108.88028169014109</v>
+        <v>106.88028169014108</v>
       </c>
       <c r="J33" t="n">
         <v>100.88028169014102</v>
@@ -14912,10 +14912,10 @@
         <v>0.0673465148754811</v>
       </c>
       <c r="L33" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M33" t="n">
-        <v>0.07074396468969091</v>
+        <v>0.07072066180141802</v>
       </c>
     </row>
     <row r="34">
@@ -14948,7 +14948,7 @@
         <v>0.0</v>
       </c>
       <c r="I34" t="n">
-        <v>317.5070422535198</v>
+        <v>315.5070422535199</v>
       </c>
       <c r="J34" t="n">
         <v>309.5070422535201</v>
@@ -14957,10 +14957,10 @@
         <v>0.11347199999999998</v>
       </c>
       <c r="L34" t="n">
-        <v>0.00302665297978472</v>
+        <v>0.0030112038806481716</v>
       </c>
       <c r="M34" t="n">
-        <v>0.11649865297978469</v>
+        <v>0.11648320388064815</v>
       </c>
     </row>
     <row r="35">
@@ -14993,7 +14993,7 @@
         <v>0.0</v>
       </c>
       <c r="I35" t="n">
-        <v>317.5070422535198</v>
+        <v>315.5070422535199</v>
       </c>
       <c r="J35" t="n">
         <v>309.5070422535201</v>
@@ -15002,10 +15002,10 @@
         <v>0.061613305263157885</v>
       </c>
       <c r="L35" t="n">
-        <v>0.00302665297978472</v>
+        <v>0.0030112038806481716</v>
       </c>
       <c r="M35" t="n">
-        <v>0.06463995824294261</v>
+        <v>0.06462450914380606</v>
       </c>
     </row>
     <row r="36">
@@ -15083,7 +15083,7 @@
         <v>0.0</v>
       </c>
       <c r="I37" t="n">
-        <v>318.03521126760427</v>
+        <v>316.0352112676044</v>
       </c>
       <c r="J37" t="n">
         <v>310.0352112676046</v>
@@ -15092,10 +15092,10 @@
         <v>0.10227442708333333</v>
       </c>
       <c r="L37" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M37" t="n">
-        <v>0.10567187689754313</v>
+        <v>0.10564857400927025</v>
       </c>
     </row>
     <row r="38">
@@ -15128,7 +15128,7 @@
         <v>0.0</v>
       </c>
       <c r="I38" t="n">
-        <v>108.35211267605658</v>
+        <v>106.35211267605656</v>
       </c>
       <c r="J38" t="n">
         <v>100.3521126760565</v>
@@ -15137,10 +15137,10 @@
         <v>0.0673465148754811</v>
       </c>
       <c r="L38" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M38" t="n">
-        <v>0.07074396468969091</v>
+        <v>0.07072066180141802</v>
       </c>
     </row>
     <row r="39">
@@ -15173,7 +15173,7 @@
         <v>0.0</v>
       </c>
       <c r="I39" t="n">
-        <v>318.03521126760427</v>
+        <v>316.0352112676044</v>
       </c>
       <c r="J39" t="n">
         <v>310.0352112676046</v>
@@ -15182,10 +15182,10 @@
         <v>0.11347199999999998</v>
       </c>
       <c r="L39" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
       <c r="M39" t="n">
-        <v>0.11649607271296476</v>
+        <v>0.11648063678441571</v>
       </c>
     </row>
     <row r="40">
@@ -15218,7 +15218,7 @@
         <v>0.0</v>
       </c>
       <c r="I40" t="n">
-        <v>317.5070422535198</v>
+        <v>315.5070422535199</v>
       </c>
       <c r="J40" t="n">
         <v>309.5070422535201</v>
@@ -15227,10 +15227,10 @@
         <v>0.061613305263157885</v>
       </c>
       <c r="L40" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
       <c r="M40" t="n">
-        <v>0.06463737797612266</v>
+        <v>0.06462194204757361</v>
       </c>
     </row>
     <row r="41">
@@ -15308,7 +15308,7 @@
         <v>0.0</v>
       </c>
       <c r="I42" t="n">
-        <v>318.56338028168875</v>
+        <v>316.56338028168886</v>
       </c>
       <c r="J42" t="n">
         <v>310.5633802816891</v>
@@ -15317,10 +15317,10 @@
         <v>0.10227442708333333</v>
       </c>
       <c r="L42" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M42" t="n">
-        <v>0.10567187689754313</v>
+        <v>0.10564857400927025</v>
       </c>
     </row>
     <row r="43">
@@ -15353,7 +15353,7 @@
         <v>0.0</v>
       </c>
       <c r="I43" t="n">
-        <v>107.82394366197207</v>
+        <v>105.82394366197205</v>
       </c>
       <c r="J43" t="n">
         <v>99.823943661972</v>
@@ -15362,10 +15362,10 @@
         <v>0.0673465148754811</v>
       </c>
       <c r="L43" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M43" t="n">
-        <v>0.07074396468969091</v>
+        <v>0.07072066180141802</v>
       </c>
     </row>
     <row r="44">
@@ -15398,7 +15398,7 @@
         <v>0.0</v>
       </c>
       <c r="I44" t="n">
-        <v>318.56338028168875</v>
+        <v>316.56338028168886</v>
       </c>
       <c r="J44" t="n">
         <v>310.5633802816891</v>
@@ -15407,10 +15407,10 @@
         <v>0.11347199999999998</v>
       </c>
       <c r="L44" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
       <c r="M44" t="n">
-        <v>0.11649607271296476</v>
+        <v>0.11648063678441571</v>
       </c>
     </row>
     <row r="45">
@@ -15443,7 +15443,7 @@
         <v>0.0</v>
       </c>
       <c r="I45" t="n">
-        <v>316.9788732394353</v>
+        <v>314.9788732394354</v>
       </c>
       <c r="J45" t="n">
         <v>308.97887323943564</v>
@@ -15452,10 +15452,10 @@
         <v>0.061613305263157885</v>
       </c>
       <c r="L45" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
       <c r="M45" t="n">
-        <v>0.06463737797612266</v>
+        <v>0.06462194204757361</v>
       </c>
     </row>
     <row r="46">
@@ -15533,7 +15533,7 @@
         <v>0.0</v>
       </c>
       <c r="I47" t="n">
-        <v>319.09154929577323</v>
+        <v>317.09154929577335</v>
       </c>
       <c r="J47" t="n">
         <v>311.0915492957736</v>
@@ -15542,10 +15542,10 @@
         <v>0.10227442708333333</v>
       </c>
       <c r="L47" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M47" t="n">
-        <v>0.10567187689754313</v>
+        <v>0.10564857400927025</v>
       </c>
     </row>
     <row r="48">
@@ -15578,7 +15578,7 @@
         <v>0.0</v>
       </c>
       <c r="I48" t="n">
-        <v>107.29577464788755</v>
+        <v>105.29577464788754</v>
       </c>
       <c r="J48" t="n">
         <v>99.29577464788748</v>
@@ -15587,10 +15587,10 @@
         <v>0.0673465148754811</v>
       </c>
       <c r="L48" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M48" t="n">
-        <v>0.07074396468969091</v>
+        <v>0.07072066180141802</v>
       </c>
     </row>
     <row r="49">
@@ -15623,7 +15623,7 @@
         <v>0.0</v>
       </c>
       <c r="I49" t="n">
-        <v>319.09154929577323</v>
+        <v>317.09154929577335</v>
       </c>
       <c r="J49" t="n">
         <v>311.0915492957736</v>
@@ -15632,10 +15632,10 @@
         <v>0.11347199999999998</v>
       </c>
       <c r="L49" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
       <c r="M49" t="n">
-        <v>0.11649607271296476</v>
+        <v>0.11648063678441571</v>
       </c>
     </row>
     <row r="50">
@@ -15668,7 +15668,7 @@
         <v>0.0</v>
       </c>
       <c r="I50" t="n">
-        <v>316.4507042253508</v>
+        <v>314.45070422535093</v>
       </c>
       <c r="J50" t="n">
         <v>308.45070422535116</v>
@@ -15677,10 +15677,10 @@
         <v>0.061613305263157885</v>
       </c>
       <c r="L50" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
       <c r="M50" t="n">
-        <v>0.06463737797612266</v>
+        <v>0.06462194204757361</v>
       </c>
     </row>
     <row r="51">
@@ -15758,7 +15758,7 @@
         <v>0.0</v>
       </c>
       <c r="I52" t="n">
-        <v>319.09154929577323</v>
+        <v>317.09154929577335</v>
       </c>
       <c r="J52" t="n">
         <v>311.0915492957736</v>
@@ -15767,10 +15767,10 @@
         <v>0.10227442708333333</v>
       </c>
       <c r="L52" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M52" t="n">
-        <v>0.10567187689754313</v>
+        <v>0.10564857400927025</v>
       </c>
     </row>
     <row r="53">
@@ -15803,7 +15803,7 @@
         <v>0.0</v>
       </c>
       <c r="I53" t="n">
-        <v>107.29577464788755</v>
+        <v>105.29577464788754</v>
       </c>
       <c r="J53" t="n">
         <v>99.29577464788748</v>
@@ -15812,10 +15812,10 @@
         <v>0.0673465148754811</v>
       </c>
       <c r="L53" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M53" t="n">
-        <v>0.07074396468969091</v>
+        <v>0.07072066180141802</v>
       </c>
     </row>
     <row r="54">
@@ -15848,7 +15848,7 @@
         <v>0.0</v>
       </c>
       <c r="I54" t="n">
-        <v>319.09154929577323</v>
+        <v>317.09154929577335</v>
       </c>
       <c r="J54" t="n">
         <v>311.0915492957736</v>
@@ -15857,10 +15857,10 @@
         <v>0.11347199999999998</v>
       </c>
       <c r="L54" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
       <c r="M54" t="n">
-        <v>0.11649607271296476</v>
+        <v>0.11648063678441571</v>
       </c>
     </row>
     <row r="55">
@@ -15893,7 +15893,7 @@
         <v>0.0</v>
       </c>
       <c r="I55" t="n">
-        <v>316.4507042253508</v>
+        <v>314.45070422535093</v>
       </c>
       <c r="J55" t="n">
         <v>308.45070422535116</v>
@@ -15902,10 +15902,10 @@
         <v>0.061613305263157885</v>
       </c>
       <c r="L55" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
       <c r="M55" t="n">
-        <v>0.06463737797612266</v>
+        <v>0.06462194204757361</v>
       </c>
     </row>
     <row r="56">
@@ -15983,7 +15983,7 @@
         <v>0.0</v>
       </c>
       <c r="I57" t="n">
-        <v>318.56338028168875</v>
+        <v>316.56338028168886</v>
       </c>
       <c r="J57" t="n">
         <v>310.5633802816891</v>
@@ -15992,10 +15992,10 @@
         <v>0.10227442708333333</v>
       </c>
       <c r="L57" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M57" t="n">
-        <v>0.10567187689754313</v>
+        <v>0.10564857400927025</v>
       </c>
     </row>
     <row r="58">
@@ -16028,7 +16028,7 @@
         <v>0.0</v>
       </c>
       <c r="I58" t="n">
-        <v>107.82394366197207</v>
+        <v>105.82394366197205</v>
       </c>
       <c r="J58" t="n">
         <v>99.823943661972</v>
@@ -16037,10 +16037,10 @@
         <v>0.0673465148754811</v>
       </c>
       <c r="L58" t="n">
-        <v>0.0033974498142098136</v>
+        <v>0.0033741469259369254</v>
       </c>
       <c r="M58" t="n">
-        <v>0.07074396468969091</v>
+        <v>0.07072066180141802</v>
       </c>
     </row>
     <row r="59">
@@ -16073,7 +16073,7 @@
         <v>0.0</v>
       </c>
       <c r="I59" t="n">
-        <v>318.56338028168875</v>
+        <v>316.56338028168886</v>
       </c>
       <c r="J59" t="n">
         <v>310.5633802816891</v>
@@ -16082,10 +16082,10 @@
         <v>0.11347199999999998</v>
       </c>
       <c r="L59" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
       <c r="M59" t="n">
-        <v>0.11649607271296476</v>
+        <v>0.11648063678441571</v>
       </c>
     </row>
     <row r="60">
@@ -16118,7 +16118,7 @@
         <v>0.0</v>
       </c>
       <c r="I60" t="n">
-        <v>316.9788732394353</v>
+        <v>314.9788732394354</v>
       </c>
       <c r="J60" t="n">
         <v>308.97887323943564</v>
@@ -16127,10 +16127,10 @@
         <v>0.061613305263157885</v>
       </c>
       <c r="L60" t="n">
-        <v>0.003024072712964784</v>
+        <v>0.0030086367844157354</v>
       </c>
       <c r="M60" t="n">
-        <v>0.06463737797612266</v>
+        <v>0.06462194204757361</v>
       </c>
     </row>
     <row r="61">
@@ -27454,7 +27454,7 @@
         <v>3.46608E7</v>
       </c>
       <c r="F10" t="n">
-        <v>109724.58970312076</v>
+        <v>109724.58970312064</v>
       </c>
       <c r="G10" t="n">
         <v>269280.0</v>
@@ -27799,7 +27799,7 @@
         <v>3.39648E7</v>
       </c>
       <c r="F25" t="n">
-        <v>112091.76911818422</v>
+        <v>112091.76911818427</v>
       </c>
       <c r="G25" t="n">
         <v>533040.0</v>
@@ -27819,10 +27819,10 @@
         <v>0.0</v>
       </c>
       <c r="E26" t="n">
-        <v>3.21552E7</v>
+        <v>3.19824E7</v>
       </c>
       <c r="F26" t="n">
-        <v>102681.06566900048</v>
+        <v>102539.86466900057</v>
       </c>
       <c r="G26" t="n">
         <v>3453120.0</v>
@@ -28167,7 +28167,7 @@
         <v>3.543E7</v>
       </c>
       <c r="F41" t="n">
-        <v>114798.21879059813</v>
+        <v>114798.2187905979</v>
       </c>
       <c r="G41" t="n">
         <v>308400.0</v>
@@ -28187,13 +28187,13 @@
         <v>0.0</v>
       </c>
       <c r="E42" t="n">
-        <v>3.3672E7</v>
+        <v>3.36912E7</v>
       </c>
       <c r="F42" t="n">
-        <v>106679.36416482659</v>
+        <v>107235.6567227214</v>
       </c>
       <c r="G42" t="n">
-        <v>3307680.0</v>
+        <v>3115680.0</v>
       </c>
     </row>
     <row r="43">
@@ -28532,13 +28532,13 @@
         <v>0.0</v>
       </c>
       <c r="E57" t="n">
-        <v>3.2136E7</v>
+        <v>3.2328E7</v>
       </c>
       <c r="F57" t="n">
-        <v>101099.41570166862</v>
+        <v>101796.90925956325</v>
       </c>
       <c r="G57" t="n">
-        <v>4745520.0</v>
+        <v>4553520.0</v>
       </c>
     </row>
     <row r="58">
@@ -28555,13 +28555,13 @@
         <v>0.0</v>
       </c>
       <c r="E58" t="n">
-        <v>3.62268E7</v>
+        <v>3.6246E7</v>
       </c>
       <c r="F58" t="n">
-        <v>113044.52113324794</v>
+        <v>113600.81369114251</v>
       </c>
       <c r="G58" t="n">
-        <v>1765200.0</v>
+        <v>1573200.0</v>
       </c>
     </row>
     <row r="59">
@@ -28900,10 +28900,10 @@
         <v>0.0</v>
       </c>
       <c r="E73" t="n">
-        <v>3.08496E7</v>
+        <v>3.06768E7</v>
       </c>
       <c r="F73" t="n">
-        <v>102751.27049114229</v>
+        <v>102610.06949114213</v>
       </c>
       <c r="G73" t="n">
         <v>3797040.0</v>
@@ -28923,10 +28923,10 @@
         <v>0.0</v>
       </c>
       <c r="E74" t="n">
-        <v>3.49008E7</v>
+        <v>3.47088E7</v>
       </c>
       <c r="F74" t="n">
-        <v>117954.92776482689</v>
+        <v>117257.43420693185</v>
       </c>
       <c r="G74" t="n">
         <v>620880.0</v>
@@ -29268,10 +29268,10 @@
         <v>0.0</v>
       </c>
       <c r="E89" t="n">
-        <v>3.32496E7</v>
+        <v>3.30768E7</v>
       </c>
       <c r="F89" t="n">
-        <v>109037.22395430043</v>
+        <v>108896.02295430041</v>
       </c>
       <c r="G89" t="n">
         <v>1903920.0</v>
@@ -29291,13 +29291,13 @@
         <v>0.0</v>
       </c>
       <c r="E90" t="n">
-        <v>3.13488E7</v>
+        <v>3.15408E7</v>
       </c>
       <c r="F90" t="n">
-        <v>102618.58093324742</v>
+        <v>103316.07449114224</v>
       </c>
       <c r="G90" t="n">
-        <v>4088400.0</v>
+        <v>3896400.0</v>
       </c>
     </row>
     <row r="91">
@@ -29650,10 +29650,10 @@
         <v>4.0</v>
       </c>
       <c r="C11" t="n">
-        <v>8812800.0</v>
+        <v>8985600.0</v>
       </c>
       <c r="D11" t="n">
-        <v>113991.018765</v>
+        <v>116226.13678</v>
       </c>
     </row>
     <row r="12">
@@ -29730,10 +29730,10 @@
         <v>5.0</v>
       </c>
       <c r="C16" t="n">
-        <v>1.24416E7</v>
+        <v>1.22688E7</v>
       </c>
       <c r="D16" t="n">
-        <v>160928.49708000018</v>
+        <v>158693.37906500016</v>
       </c>
     </row>
     <row r="17">
@@ -29861,7 +29861,7 @@
         <v>1.032192E7</v>
       </c>
       <c r="D24" t="n">
-        <v>91751.01859839997</v>
+        <v>91751.0185984</v>
       </c>
     </row>
     <row r="25">
@@ -30114,10 +30114,10 @@
         <v>9.0</v>
       </c>
       <c r="C40" t="n">
-        <v>9676800.0</v>
+        <v>9849600.0</v>
       </c>
       <c r="D40" t="n">
-        <v>125166.60884</v>
+        <v>127401.726855</v>
       </c>
     </row>
     <row r="41">
@@ -30162,10 +30162,10 @@
         <v>10.0</v>
       </c>
       <c r="C43" t="n">
-        <v>1.07136E7</v>
+        <v>1.05408E7</v>
       </c>
       <c r="D43" t="n">
-        <v>138577.31693000003</v>
+        <v>136342.19891500002</v>
       </c>
     </row>
     <row r="44">
@@ -30210,10 +30210,10 @@
         <v>11.0</v>
       </c>
       <c r="C46" t="n">
-        <v>9676800.0</v>
+        <v>9849600.0</v>
       </c>
       <c r="D46" t="n">
-        <v>125166.60884</v>
+        <v>127401.726855</v>
       </c>
     </row>
     <row r="47">
@@ -30277,7 +30277,7 @@
         <v>1.069056E7</v>
       </c>
       <c r="D50" t="n">
-        <v>95027.84069120002</v>
+        <v>95027.84069120004</v>
       </c>
     </row>
     <row r="51">
@@ -30290,10 +30290,10 @@
         <v>12.0</v>
       </c>
       <c r="C51" t="n">
-        <v>1.07136E7</v>
+        <v>1.05408E7</v>
       </c>
       <c r="D51" t="n">
-        <v>138577.31693000003</v>
+        <v>136342.19891500002</v>
       </c>
     </row>
     <row r="52">

</xml_diff>